<commit_message>
Fixed the Excel sheet file path code to save the sheet in the same file as the script.
</commit_message>
<xml_diff>
--- a/roundData.xlsx
+++ b/roundData.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B654"/>
+  <dimension ref="A1:B655"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2906,7 +2906,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Eric Barnett , (Wisconsin) DEC Sam Latona , (Virginia Tech), 7-3</t>
+          <t>Patrick Mckee , (Minnesota) F Killian Cardinale , (West Virginia), 3:25</t>
         </is>
       </c>
     </row>
@@ -2918,7 +2918,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Michael Deaugustino , (Northwestern) DEC Joey Prata , (Oklahoma), 2-0</t>
+          <t>Eric Barnett , (Wisconsin) DEC Sam Latona , (Virginia Tech), 7-3</t>
         </is>
       </c>
     </row>
@@ -2930,19 +2930,19 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Brandon Kaylor , (Oregon State) F Noah Surtin , (Missouri), 5:31</t>
+          <t>Michael Deaugustino , (Northwestern) DEC Joey Prata , (Oklahoma), 2-0</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>125</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Korbin Myers , (Virginia Tech) MD Matt Ramos , (Purdue), 12-2</t>
+          <t>Brandon Kaylor , (Oregon State) F Noah Surtin , (Missouri), 5:31</t>
         </is>
       </c>
     </row>
@@ -2954,7 +2954,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Devan Turner , (Oregon State) DEC Brian Courtney , (Virginia), 8-4</t>
+          <t>Korbin Myers , (Virginia Tech) MD Matt Ramos , (Purdue), 12-2</t>
         </is>
       </c>
     </row>
@@ -2966,7 +2966,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Chris Cannon , (Northwestern) F Micky Phillippi , (Pittsburgh), 2:21</t>
+          <t>Devan Turner , (Oregon State) DEC Brian Courtney , (Virginia), 8-4</t>
         </is>
       </c>
     </row>
@@ -2978,19 +2978,19 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Lucas Byrd , (Illinois) DEC Dylan Ragusin , (Michigan), 6-5</t>
+          <t>Chris Cannon , (Northwestern) F Micky Phillippi , (Pittsburgh), 2:21</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>133</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Cj Composto , (Penn) DEC Stevan Micic , (Michigan), 10-4 SV</t>
+          <t>Lucas Byrd , (Illinois) DEC Dylan Ragusin , (Michigan), 6-5</t>
         </is>
       </c>
     </row>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Grant Willits , (Oregon State) F Chad Red , (Nebraska), 3:45</t>
+          <t>Cj Composto , (Penn) DEC Stevan Micic , (Michigan), 10-4 SV</t>
         </is>
       </c>
     </row>
@@ -3014,7 +3014,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Jake Bergeland , (Minnesota) F Andrew Alirez , (Northern Colorado), 2:35</t>
+          <t>Grant Willits , (Oregon State) F Chad Red , (Nebraska), 3:45</t>
         </is>
       </c>
     </row>
@@ -3026,19 +3026,19 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Sebastian Rivera , (Rutgers) DEC Clay Carlson , (South Dakota State), 6-2</t>
+          <t>Jake Bergeland , (Minnesota) F Andrew Alirez , (Northern Colorado), 2:35</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>141</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Kyle Parco , (Arizona State) DEC Anthony Artalona , (Penn), 3-2</t>
+          <t>Sebastian Rivera , (Rutgers) DEC Clay Carlson , (South Dakota State), 6-2</t>
         </is>
       </c>
     </row>
@@ -3050,7 +3050,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Jonathan Millner , (Appalachian State) DEC Max Murin , (Iowa), 8-1</t>
+          <t>Kyle Parco , (Arizona State) DEC Anthony Artalona , (Penn), 3-2</t>
         </is>
       </c>
     </row>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Tariq Wilson , (NC State) DEC Yahya Thomas , (Northwestern), 9-5</t>
+          <t>Jonathan Millner , (Appalachian State) DEC Max Murin , (Iowa), 8-1</t>
         </is>
       </c>
     </row>
@@ -3074,19 +3074,19 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Austin Gomez , (Wisconsin) DEC Kaden Gfeller , (Oklahoma State), 7-4</t>
+          <t>Tariq Wilson , (NC State) DEC Yahya Thomas , (Northwestern), 9-5</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>149</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Peyton Robb , (Nebraska) F Ed Scott , (NC State), 4:36</t>
+          <t>Austin Gomez , (Wisconsin) DEC Kaden Gfeller , (Oklahoma State), 7-4</t>
         </is>
       </c>
     </row>
@@ -3098,7 +3098,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Hunter Willits , (Oregon State) DEC Dazjon Casto , (The Citadel), 7-6</t>
+          <t>Peyton Robb , (Nebraska) F Ed Scott , (NC State), 4:36</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Austin O`connor , (North Carolina) DEC Josh Humphreys , (Lehigh), 4-3</t>
+          <t>Hunter Willits , (Oregon State) DEC Dazjon Casto , (The Citadel), 7-6</t>
         </is>
       </c>
     </row>
@@ -3122,19 +3122,19 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>David Carr , (Iowa State) DEC Jared Franek , (North Dakota State), 4-3</t>
+          <t>Austin O`connor , (North Carolina) DEC Josh Humphreys , (Lehigh), 4-3</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>157</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Dean Hamiti , (Wisconsin) MD Jake Wentzel , (Pittsburgh), 8-0</t>
+          <t>David Carr , (Iowa State) DEC Jared Franek , (North Dakota State), 4-3</t>
         </is>
       </c>
     </row>
@@ -3146,7 +3146,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Peyton Hall , (West Virginia) MD Justin Mccoy , (Virginia), 11-3</t>
+          <t>Dean Hamiti , (Wisconsin) MD Jake Wentzel , (Pittsburgh), 8-0</t>
         </is>
       </c>
     </row>
@@ -3158,7 +3158,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Carson Kharchla , (Ohio State) DEC Julian Ramirez , (Cornell), 4-3</t>
+          <t>Peyton Hall , (West Virginia) MD Justin Mccoy , (Virginia), 11-3</t>
         </is>
       </c>
     </row>
@@ -3170,19 +3170,19 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Alex Marinelli , (Iowa) DEC Philip Conigliaro , (Harvard), 6-2</t>
+          <t>Carson Kharchla , (Ohio State) DEC Julian Ramirez , (Cornell), 4-3</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>174</t>
+          <t>165</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Michael Kemerer , (Iowa) DEC Michael O'malley Hasbrouck Heights, NJ (Drexel), 5-2</t>
+          <t>Alex Marinelli , (Iowa) DEC Philip Conigliaro , (Harvard), 6-2</t>
         </is>
       </c>
     </row>
@@ -3194,7 +3194,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Mikey Labriola , (Nebraska) DEC Hayden Hastings , (Wyoming), 5-3</t>
+          <t>Michael Kemerer , (Iowa) DEC Michael O'malley Hasbrouck Heights, NJ (Drexel), 5-2</t>
         </is>
       </c>
     </row>
@@ -3206,7 +3206,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Clay Lautt , (North Carolina) DEC Peyton Mocco , (Missouri), 6-3</t>
+          <t>Mikey Labriola , (Nebraska) DEC Hayden Hastings , (Wyoming), 5-3</t>
         </is>
       </c>
     </row>
@@ -3218,19 +3218,19 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Dustin Plott , (Oklahoma State) DEC Ethan Smith , (Ohio State), 9-7 SV</t>
+          <t>Clay Lautt , (North Carolina) DEC Peyton Mocco , (Missouri), 6-3</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>184</t>
+          <t>174</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Parker Keckeisen , (Northern Iowa) DEC Taylor Venz , (Nebraska), 7-5</t>
+          <t>Dustin Plott , (Oklahoma State) DEC Ethan Smith , (Ohio State), 9-7 SV</t>
         </is>
       </c>
     </row>
@@ -3242,7 +3242,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Jonathan Loew , (Cornell) DEC Zach Braunagel , (Illinois), 3-1 SV</t>
+          <t>Parker Keckeisen , (Northern Iowa) DEC Taylor Venz , (Nebraska), 7-5</t>
         </is>
       </c>
     </row>
@@ -3254,7 +3254,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Kaleb Romero , (Ohio State) MD Max Lyon , (Purdue), 15-6</t>
+          <t>Jonathan Loew , (Cornell) DEC Zach Braunagel , (Illinois), 3-1 SV</t>
         </is>
       </c>
     </row>
@@ -3266,19 +3266,19 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Marcus Coleman , (Iowa State) MD Trey Munoz , (Oregon State), 13-2</t>
+          <t>Kaleb Romero , (Ohio State) MD Max Lyon , (Purdue), 15-6</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>197</t>
+          <t>184</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Yonger Bastida , (Iowa State) DEC Jake Woodley , (Oklahoma), 5-4</t>
+          <t>Marcus Coleman , (Iowa State) MD Trey Munoz , (Oregon State), 13-2</t>
         </is>
       </c>
     </row>
@@ -3290,7 +3290,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Greg Bulsak , (Rutgers) DEC Lou Deprez , (Binghamton), 3-2</t>
+          <t>Yonger Bastida , (Iowa State) DEC Jake Woodley , (Oklahoma), 5-4</t>
         </is>
       </c>
     </row>
@@ -3302,7 +3302,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Rocky Elam , (Missouri) DEC Nino Bonaccorsi , (Pittsburgh), 6-1</t>
+          <t>Greg Bulsak , (Rutgers) DEC Lou Deprez , (Binghamton), 3-2</t>
         </is>
       </c>
     </row>
@@ -3314,19 +3314,19 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Eric Schultz , (Nebraska) DEC Jay Aiello , (Virginia), 4-2</t>
+          <t>Rocky Elam , (Missouri) DEC Nino Bonaccorsi , (Pittsburgh), 6-1</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>285</t>
+          <t>197</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Christian Lance , (Nebraska) DEC Lewis Fernandes , (Cornell), 4-2 SV</t>
+          <t>Eric Schultz , (Nebraska) DEC Jay Aiello , (Virginia), 4-2</t>
         </is>
       </c>
     </row>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Lucas Davison , (Northwestern) DEC Gary Traub , (Oregon State), 8-2</t>
+          <t>Christian Lance , (Nebraska) DEC Lewis Fernandes , (Cornell), 4-2 SV</t>
         </is>
       </c>
     </row>
@@ -3350,7 +3350,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Mason Parris , (Michigan) MD Tate Orndorff , (Ohio State), 12-1</t>
+          <t>Lucas Davison , (Northwestern) DEC Gary Traub , (Oregon State), 8-2</t>
         </is>
       </c>
     </row>
@@ -3362,26 +3362,26 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Tony Cassioppi , (Iowa) DEC Zach Elam , (Missouri), 4-0</t>
+          <t>Mason Parris , (Michigan) MD Tate Orndorff , (Ohio State), 12-1</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>ROUND OF 16</t>
+          <t>285</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Tony Cassioppi , (Iowa) DEC Zach Elam , (Missouri), 4-0</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>125</t>
-        </is>
-      </c>
-      <c r="B252" t="inlineStr">
-        <is>
-          <t>Nick Suriano , (Michigan) DEC Anthony Noto , (Lock Haven), 8-3</t>
+          <t>ROUND OF 16</t>
         </is>
       </c>
     </row>
@@ -3393,7 +3393,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Sam Latona , (Virginia Tech) DEC Caleb Smith , (Appalachian State), 6-2</t>
+          <t>Nick Suriano , (Michigan) DEC Anthony Noto , (Lock Haven), 8-3</t>
         </is>
       </c>
     </row>
@@ -3405,7 +3405,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Killian Cardinale , (West Virginia) DEC Taylor Lamont , (Utah Valley), 10-8</t>
+          <t>Sam Latona , (Virginia Tech) DEC Caleb Smith , (Appalachian State), 6-2</t>
         </is>
       </c>
     </row>
@@ -3417,7 +3417,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Brandon Courtney , (Arizona State) MD Fabian Gutierrez , (Chattanooga), 12-3</t>
+          <t>Killian Cardinale , (West Virginia) DEC Taylor Lamont , (Utah Valley), 10-8</t>
         </is>
       </c>
     </row>
@@ -3429,7 +3429,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Pat Glory , (Princeton) MD Jakob Camacho , (NC State), 10-2</t>
+          <t>Brandon Courtney , (Arizona State) MD Fabian Gutierrez , (Chattanooga), 12-3</t>
         </is>
       </c>
     </row>
@@ -3441,7 +3441,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Brandon Kaylor , (Oregon State) DEC Eric Barnett , (Wisconsin), 9-3</t>
+          <t>Pat Glory , (Princeton) MD Jakob Camacho , (NC State), 10-2</t>
         </is>
       </c>
     </row>
@@ -3453,7 +3453,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Michael Deaugustino , (Northwestern) DEC Trevor Mastrogiovanni , (Oklahoma State), 3-2</t>
+          <t>Brandon Kaylor , (Oregon State) DEC Eric Barnett , (Wisconsin), 9-3</t>
         </is>
       </c>
     </row>
@@ -3465,19 +3465,19 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Vitali Arujau , (Cornell) MD Brody Teske , (Northern Iowa), 16-4</t>
+          <t>Michael Deaugustino , (Northwestern) DEC Trevor Mastrogiovanni , (Oklahoma State), 3-2</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>125</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Roman Bravo-young , (Penn State) F Joshua Koderhandt , (Navy), 4:46</t>
+          <t>Vitali Arujau , (Cornell) MD Brody Teske , (Northern Iowa), 16-4</t>
         </is>
       </c>
     </row>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Brian Courtney , (Virginia) DEC Michael Colaiocco , (Penn), 8-7</t>
+          <t>Roman Bravo-young , (Penn State) F Joshua Koderhandt , (Navy), 4:46</t>
         </is>
       </c>
     </row>
@@ -3501,7 +3501,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Austin Desanto , (Iowa) DEC Micky Phillippi , (Pittsburgh), 5-2</t>
+          <t>Brian Courtney , (Virginia) DEC Michael Colaiocco , (Penn), 8-7</t>
         </is>
       </c>
     </row>
@@ -3513,7 +3513,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Korbin Myers , (Virginia Tech) DEF Brock Hudkins , (Indiana)</t>
+          <t>Austin Desanto , (Iowa) DEC Micky Phillippi , (Pittsburgh), 5-2</t>
         </is>
       </c>
     </row>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Michael Mcgee , (Arizona State) DEC Kyle Biscoglia , (Northern Iowa), 10-4</t>
+          <t>Korbin Myers , (Virginia Tech) DEF Brock Hudkins , (Indiana)</t>
         </is>
       </c>
     </row>
@@ -3537,7 +3537,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Dylan Ragusin , (Michigan) DEC Devan Turner , (Oregon State), 4-2</t>
+          <t>Michael Mcgee , (Arizona State) DEC Kyle Biscoglia , (Northern Iowa), 10-4</t>
         </is>
       </c>
     </row>
@@ -3549,7 +3549,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Chris Cannon , (Northwestern) DEC Matt Ramos , (Purdue), 1-0</t>
+          <t>Dylan Ragusin , (Michigan) DEC Devan Turner , (Oregon State), 4-2</t>
         </is>
       </c>
     </row>
@@ -3561,19 +3561,19 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Daton Fix , (Oklahoma State) DEC Kai Orine , (NC State), 7-4</t>
+          <t>Chris Cannon , (Northwestern) DEC Matt Ramos , (Purdue), 1-0</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>133</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Nick Lee , (Penn State) DEC Quinn Kinner , (Rider), 9-2</t>
+          <t>Daton Fix , (Oklahoma State) DEC Kai Orine , (NC State), 7-4</t>
         </is>
       </c>
     </row>
@@ -3585,7 +3585,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Grant Willits , (Oregon State) DEC Allan Hart , (Missouri), 3-1</t>
+          <t>Nick Lee , (Penn State) DEC Quinn Kinner , (Rider), 9-2</t>
         </is>
       </c>
     </row>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Cj Composto , (Penn) DEC Andrew Alirez , (Northern Colorado), 5-4</t>
+          <t>Grant Willits , (Oregon State) DEC Allan Hart , (Missouri), 3-1</t>
         </is>
       </c>
     </row>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Real Woods , (Stanford) MD Parker Filius , (Purdue), 8-0</t>
+          <t>Cj Composto , (Penn) DEC Andrew Alirez , (Northern Colorado), 5-4</t>
         </is>
       </c>
     </row>
@@ -3621,7 +3621,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Sebastian Rivera , (Rutgers) DEC Chad Red , (Nebraska), 7-6</t>
+          <t>Real Woods , (Stanford) MD Parker Filius , (Purdue), 8-0</t>
         </is>
       </c>
     </row>
@@ -3633,7 +3633,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Cole Matthews , (Pittsburgh) DEC Matt Kazimir , (Columbia), 3-2</t>
+          <t>Sebastian Rivera , (Rutgers) DEC Chad Red , (Nebraska), 7-6</t>
         </is>
       </c>
     </row>
@@ -3645,7 +3645,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Jake Bergeland , (Minnesota) DEC Frankie Tal sharar , (Northwestern), 5-3</t>
+          <t>Cole Matthews , (Pittsburgh) DEC Matt Kazimir , (Columbia), 3-2</t>
         </is>
       </c>
     </row>
@@ -3657,19 +3657,19 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Kizhan Clarke , (North Carolina) DEC Jaydin Eierman , (Iowa), 4-2</t>
+          <t>Jake Bergeland , (Minnesota) DEC Frankie Tal sharar , (Northwestern), 5-3</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>141</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Yianni Diakomihalis , (Cornell) DEC Willie Mcdougald , (Oklahoma), 11-5</t>
+          <t>Kizhan Clarke , (North Carolina) DEC Jaydin Eierman , (Iowa), 4-2</t>
         </is>
       </c>
     </row>
@@ -3681,7 +3681,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Max Murin , (Iowa) DEC Kaden Gfeller , (Oklahoma State), 8-4</t>
+          <t>Yianni Diakomihalis , (Cornell) DEC Willie Mcdougald , (Oklahoma), 11-5</t>
         </is>
       </c>
     </row>
@@ -3693,7 +3693,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Kyle Parco , (Arizona State) DEC Marcus Robinson , (Cleveland State), 6-2</t>
+          <t>Max Murin , (Iowa) DEC Kaden Gfeller , (Oklahoma State), 8-4</t>
         </is>
       </c>
     </row>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Sammy Sasso , (Ohio State) DEC Beau Bartlett , (Penn State), 6-4</t>
+          <t>Kyle Parco , (Arizona State) DEC Marcus Robinson , (Cleveland State), 6-2</t>
         </is>
       </c>
     </row>
@@ -3717,7 +3717,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Austin Gomez , (Wisconsin) MD Josh Finesilver , (Duke), 19-7</t>
+          <t>Sammy Sasso , (Ohio State) DEC Beau Bartlett , (Penn State), 6-4</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Bryce Andonian , (Virginia Tech) DEC Jonathan Millner , (Appalachian State), 16-11</t>
+          <t>Austin Gomez , (Wisconsin) MD Josh Finesilver , (Duke), 19-7</t>
         </is>
       </c>
     </row>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Ridge Lovett , (Nebraska) DEC Joshua Heil , (Campbell), 8-1</t>
+          <t>Bryce Andonian , (Virginia Tech) DEC Jonathan Millner , (Appalachian State), 16-11</t>
         </is>
       </c>
     </row>
@@ -3753,19 +3753,19 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Tariq Wilson , (NC State) DEC Anthony Artalona , (Penn), 4-3</t>
+          <t>Ridge Lovett , (Nebraska) DEC Joshua Heil , (Campbell), 8-1</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>149</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Hunter Willits , (Oregon State) DEC David Carr , (Iowa State), 2-1</t>
+          <t>Tariq Wilson , (NC State) DEC Anthony Artalona , (Penn), 4-3</t>
         </is>
       </c>
     </row>
@@ -3777,7 +3777,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Will Lewan , (Michigan) DEC Kaleb Young , (Iowa), 3-1</t>
+          <t>Hunter Willits , (Oregon State) DEC David Carr , (Iowa State), 2-1</t>
         </is>
       </c>
     </row>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Quincy Monday , (Princeton) DEC Jacob Wright , (Wyoming), 3-2</t>
+          <t>Will Lewan , (Michigan) DEC Kaleb Young , (Iowa), 3-1</t>
         </is>
       </c>
     </row>
@@ -3801,7 +3801,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Ed Scott , (NC State) DEC Justin Thomas , (Oklahoma), 9-6</t>
+          <t>Quincy Monday , (Princeton) DEC Jacob Wright , (Wyoming), 3-2</t>
         </is>
       </c>
     </row>
@@ -3813,7 +3813,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Jacori Teemer , (Arizona State) F Jake Keating , (Virginia), 2:43</t>
+          <t>Ed Scott , (NC State) DEC Justin Thomas , (Oklahoma), 9-6</t>
         </is>
       </c>
     </row>
@@ -3825,7 +3825,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Jared Franek , (North Dakota State) DEC Dazjon Casto , (The Citadel), 3-2</t>
+          <t>Jacori Teemer , (Arizona State) F Jake Keating , (Virginia), 2:43</t>
         </is>
       </c>
     </row>
@@ -3837,7 +3837,7 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Josh Humphreys , (Lehigh) DEC Peyton Robb , (Nebraska), 8-5</t>
+          <t>Jared Franek , (North Dakota State) DEC Dazjon Casto , (The Citadel), 3-2</t>
         </is>
       </c>
     </row>
@@ -3849,19 +3849,19 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Ryan Deakin , (Northwestern) F Johnny Lovett , (Central Michigan), 4:36</t>
+          <t>Josh Humphreys , (Lehigh) DEC Peyton Robb , (Nebraska), 8-5</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>157</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Evan Wick , (California Poly) DEC Luke Weber , (North Dakota State), 10-5</t>
+          <t>Ryan Deakin , (Northwestern) F Johnny Lovett , (Central Michigan), 4:36</t>
         </is>
       </c>
     </row>
@@ -3873,7 +3873,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Peyton Hall , (West Virginia) DEC Philip Conigliaro , (Harvard), 7-3</t>
+          <t>Evan Wick , (California Poly) DEC Luke Weber , (North Dakota State), 10-5</t>
         </is>
       </c>
     </row>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Shane Griffith , (Stanford) DEC Zach Hartman , (Bucknell), 7-3</t>
+          <t>Peyton Hall , (West Virginia) DEC Philip Conigliaro , (Harvard), 7-3</t>
         </is>
       </c>
     </row>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Dean Hamiti , (Wisconsin) DEC Julian Ramirez , (Cornell), 15-11</t>
+          <t>Shane Griffith , (Stanford) DEC Zach Hartman , (Bucknell), 7-3</t>
         </is>
       </c>
     </row>
@@ -3909,7 +3909,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Alex Marinelli , (Iowa) DEC Justin Mccoy , (Virginia), 8-2</t>
+          <t>Dean Hamiti , (Wisconsin) DEC Julian Ramirez , (Cornell), 15-11</t>
         </is>
       </c>
     </row>
@@ -3921,7 +3921,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Cameron Amine , (Michigan) DEC Izzak Olejnik , (Northern Illinois), 4-2</t>
+          <t>Alex Marinelli , (Iowa) DEC Justin Mccoy , (Virginia), 8-2</t>
         </is>
       </c>
     </row>
@@ -3933,7 +3933,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Carson Kharchla , (Ohio State) DEC Jake Wentzel , (Pittsburgh), 7-1</t>
+          <t>Cameron Amine , (Michigan) DEC Izzak Olejnik , (Northern Illinois), 4-2</t>
         </is>
       </c>
     </row>
@@ -3945,19 +3945,19 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Keegan O`toole , (Missouri) DEC Anthony Valencia , (Arizona State), 7-0</t>
+          <t>Carson Kharchla , (Ohio State) DEC Jake Wentzel , (Pittsburgh), 7-1</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>174</t>
+          <t>165</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Carter Starocci , (Penn State) DEC Adam Kemp , (California Poly), 10-4</t>
+          <t>Keegan O`toole , (Missouri) DEC Anthony Valencia , (Arizona State), 7-0</t>
         </is>
       </c>
     </row>
@@ -3969,7 +3969,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Mikey Labriola , (Nebraska) DEC Gerrit Nijenhuis , (Purdue), 3-2</t>
+          <t>Carter Starocci , (Penn State) DEC Adam Kemp , (California Poly), 10-4</t>
         </is>
       </c>
     </row>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Michael Kemerer , (Iowa) DEC Cade Devos , (South Dakota State), 9-4</t>
+          <t>Mikey Labriola , (Nebraska) DEC Gerrit Nijenhuis , (Purdue), 3-2</t>
         </is>
       </c>
     </row>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Hayden Hidlay , (NC State) MD Matthew Finesilver , (Duke), 13-5</t>
+          <t>Michael Kemerer , (Iowa) DEC Cade Devos , (South Dakota State), 9-4</t>
         </is>
       </c>
     </row>
@@ -4005,7 +4005,7 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Logan Massa , (Michigan) MD Thomas Flitz , (Appalachian State), 15-5</t>
+          <t>Hayden Hidlay , (NC State) MD Matthew Finesilver , (Duke), 13-5</t>
         </is>
       </c>
     </row>
@@ -4017,7 +4017,7 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Dustin Plott , (Oklahoma State) DEC Mason Kauffman , (Northern Illinois), 8-2</t>
+          <t>Logan Massa , (Michigan) MD Thomas Flitz , (Appalachian State), 15-5</t>
         </is>
       </c>
     </row>
@@ -4029,7 +4029,7 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Clay Lautt , (North Carolina) MD Tyler Eischens , (Stanford), 13-4</t>
+          <t>Dustin Plott , (Oklahoma State) DEC Mason Kauffman , (Northern Illinois), 8-2</t>
         </is>
       </c>
     </row>
@@ -4041,19 +4041,19 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Mekhi Lewis , (Virginia Tech) DEC Lance Runyon , (Northern Iowa), 8-5</t>
+          <t>Clay Lautt , (North Carolina) MD Tyler Eischens , (Stanford), 13-4</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>184</t>
+          <t>174</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Myles Amine , (Michigan) DEC Dakota Geer , (Oklahoma State), 5-1</t>
+          <t>Mekhi Lewis , (Virginia Tech) DEC Lance Runyon , (Northern Iowa), 8-5</t>
         </is>
       </c>
     </row>
@@ -4065,7 +4065,7 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Zach Braunagel , (Illinois) F Marcus Coleman , (Iowa State), 6:47</t>
+          <t>Myles Amine , (Michigan) DEC Dakota Geer , (Oklahoma State), 5-1</t>
         </is>
       </c>
     </row>
@@ -4077,7 +4077,7 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Bernie Truax , (California Poly) DEC Tate Samuelson , (Wyoming), 6-2</t>
+          <t>Zach Braunagel , (Illinois) F Marcus Coleman , (Iowa State), 6:47</t>
         </is>
       </c>
     </row>
@@ -4089,7 +4089,7 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Parker Keckeisen , (Northern Iowa) DEC Kyle Cochran , (Maryland), 9-3</t>
+          <t>Bernie Truax , (California Poly) DEC Tate Samuelson , (Wyoming), 6-2</t>
         </is>
       </c>
     </row>
@@ -4101,7 +4101,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Trent Hidlay , (NC State) DEC Isaiah Salazar , (Minnesota), 5-3</t>
+          <t>Parker Keckeisen , (Northern Iowa) DEC Kyle Cochran , (Maryland), 9-3</t>
         </is>
       </c>
     </row>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Trey Munoz , (Oregon State) MD Jonathan Loew , (Cornell), 12-2</t>
+          <t>Trent Hidlay , (NC State) DEC Isaiah Salazar , (Minnesota), 5-3</t>
         </is>
       </c>
     </row>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Kaleb Romero , (Ohio State) DEC Taylor Venz , (Nebraska), 5-1</t>
+          <t>Trey Munoz , (Oregon State) MD Jonathan Loew , (Cornell), 12-2</t>
         </is>
       </c>
     </row>
@@ -4137,19 +4137,19 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Aaron Brooks , (Penn State) MD Hunter Bolen , (Virginia Tech), 9-1</t>
+          <t>Kaleb Romero , (Ohio State) DEC Taylor Venz , (Nebraska), 5-1</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>197</t>
+          <t>184</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Max Dean , (Penn State) DEC Jay Aiello , (Virginia), 4-2</t>
+          <t>Aaron Brooks , (Penn State) MD Hunter Bolen , (Virginia Tech), 9-1</t>
         </is>
       </c>
     </row>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Lou Deprez , (Binghamton) DEC Cameron Caffey , (Michigan State), 5-4</t>
+          <t>Max Dean , (Penn State) DEC Jay Aiello , (Virginia), 4-2</t>
         </is>
       </c>
     </row>
@@ -4173,7 +4173,7 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Gavin Hoffman , (Ohio State) DEC Nino Bonaccorsi , (Pittsburgh), 6-4</t>
+          <t>Lou Deprez , (Binghamton) DEC Cameron Caffey , (Michigan State), 5-4</t>
         </is>
       </c>
     </row>
@@ -4185,7 +4185,7 @@
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Jake Woodley , (Oklahoma) DEC Patrick Brucki , (Michigan), 6-3</t>
+          <t>Gavin Hoffman , (Ohio State) DEC Nino Bonaccorsi , (Pittsburgh), 6-4</t>
         </is>
       </c>
     </row>
@@ -4197,7 +4197,7 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Eric Schultz , (Nebraska) DEC Greg Bulsak , (Rutgers), 4-3</t>
+          <t>Jake Woodley , (Oklahoma) DEC Patrick Brucki , (Michigan), 6-3</t>
         </is>
       </c>
     </row>
@@ -4209,7 +4209,7 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Jacob Warner , (Iowa) DEC Thomas Penola , (Purdue), 3-1</t>
+          <t>Eric Schultz , (Nebraska) DEC Greg Bulsak , (Rutgers), 4-3</t>
         </is>
       </c>
     </row>
@@ -4221,7 +4221,7 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Rocky Elam , (Missouri) DEC Yonger Bastida , (Iowa State), 1-0</t>
+          <t>Jacob Warner , (Iowa) DEC Thomas Penola , (Purdue), 3-1</t>
         </is>
       </c>
     </row>
@@ -4233,19 +4233,19 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Stephen Buchanan , (Wyoming) DEC Luke Stout , (Princeton), 6-3</t>
+          <t>Rocky Elam , (Missouri) DEC Yonger Bastida , (Iowa State), 1-0</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>285</t>
+          <t>197</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Gable Steveson , (Minnesota) TF Zach Elam , (Missouri), 23-8</t>
+          <t>Stephen Buchanan , (Wyoming) DEC Luke Stout , (Princeton), 6-3</t>
         </is>
       </c>
     </row>
@@ -4257,7 +4257,7 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Lucas Davison , (Northwestern) DEC Matt Stencel , (Central Michigan), 9-2</t>
+          <t>Gable Steveson , (Minnesota) TF Zach Elam , (Missouri), 23-8</t>
         </is>
       </c>
     </row>
@@ -4269,7 +4269,7 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Christian Lance , (Nebraska) DEC Wyatt Hendrickson , (Air Force), 5-4</t>
+          <t>Lucas Davison , (Northwestern) DEC Matt Stencel , (Central Michigan), 9-2</t>
         </is>
       </c>
     </row>
@@ -4281,7 +4281,7 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Greg Kerkvliet , (Penn State) MD Tate Orndorff , (Ohio State), 10-1</t>
+          <t>Christian Lance , (Nebraska) DEC Wyatt Hendrickson , (Air Force), 5-4</t>
         </is>
       </c>
     </row>
@@ -4293,7 +4293,7 @@
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Tony Cassioppi , (Iowa) MD Luke Luffman , (Illinois), 12-3</t>
+          <t>Greg Kerkvliet , (Penn State) MD Tate Orndorff , (Ohio State), 10-1</t>
         </is>
       </c>
     </row>
@@ -4305,7 +4305,7 @@
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Jordan Wood , (Lehigh) DEC Gary Traub , (Oregon State), 6-0</t>
+          <t>Tony Cassioppi , (Iowa) MD Luke Luffman , (Illinois), 12-3</t>
         </is>
       </c>
     </row>
@@ -4317,7 +4317,7 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>Mason Parris , (Michigan) DEC Nathan Traxler , (Virginia Tech), 7-3</t>
+          <t>Jordan Wood , (Lehigh) DEC Gary Traub , (Oregon State), 6-0</t>
         </is>
       </c>
     </row>
@@ -4329,26 +4329,26 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>Cohlton Schultz , (Arizona State) F Lewis Fernandes , (Cornell), 0:52</t>
+          <t>Mason Parris , (Michigan) DEC Nathan Traxler , (Virginia Tech), 7-3</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>CONSI OF 16 #2</t>
+          <t>285</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Cohlton Schultz , (Arizona State) F Lewis Fernandes , (Cornell), 0:52</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>125</t>
-        </is>
-      </c>
-      <c r="B333" t="inlineStr">
-        <is>
-          <t>Brody Teske , (Northern Iowa) DEC Drew Hildebrandt , (Penn State), 8-4</t>
+          <t>CONSI OF 16 #2</t>
         </is>
       </c>
     </row>
@@ -4360,7 +4360,7 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>Patrick Mckee , (Minnesota) MD Trevor Mastrogiovanni , (Oklahoma State), 9-1</t>
+          <t>Brody Teske , (Northern Iowa) DEC Drew Hildebrandt , (Penn State), 8-4</t>
         </is>
       </c>
     </row>
@@ -4372,7 +4372,7 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>Eric Barnett , (Wisconsin) DEC Malik Heinselman , (Ohio State), 9-4</t>
+          <t>Patrick Mckee , (Minnesota) MD Trevor Mastrogiovanni , (Oklahoma State), 9-1</t>
         </is>
       </c>
     </row>
@@ -4384,7 +4384,7 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>Jakob Camacho , (NC State) DEC Drake Ayala , (Iowa), 8-5</t>
+          <t>Eric Barnett , (Wisconsin) DEC Malik Heinselman , (Ohio State), 9-4</t>
         </is>
       </c>
     </row>
@@ -4396,7 +4396,7 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>Joey Prata , (Oklahoma) DEC Fabian Gutierrez , (Chattanooga), 5-2</t>
+          <t>Jakob Camacho , (NC State) DEC Drake Ayala , (Iowa), 8-5</t>
         </is>
       </c>
     </row>
@@ -4408,7 +4408,7 @@
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>Taylor Lamont , (Utah Valley) DEC Ryan Miller , (Penn), 6-5</t>
+          <t>Joey Prata , (Oklahoma) DEC Fabian Gutierrez , (Chattanooga), 5-2</t>
         </is>
       </c>
     </row>
@@ -4420,7 +4420,7 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>Dylan Shawver , (Rutgers) DEC Caleb Smith , (Appalachian State), 10-7</t>
+          <t>Taylor Lamont , (Utah Valley) DEC Ryan Miller , (Penn), 6-5</t>
         </is>
       </c>
     </row>
@@ -4432,19 +4432,19 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>Noah Surtin , (Missouri) F Anthony Noto , (Lock Haven), 6:40</t>
+          <t>Dylan Shawver , (Rutgers) DEC Caleb Smith , (Appalachian State), 10-7</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>125</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>Kai Orine , (NC State) DEC Haiden Drury , (Utah Valley), 3-2</t>
+          <t>Noah Surtin , (Missouri) F Anthony Noto , (Lock Haven), 6:40</t>
         </is>
       </c>
     </row>
@@ -4456,7 +4456,7 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>Matt Ramos , (Purdue) DEC Rayvon Foley , (Michigan State), 9-6</t>
+          <t>Kai Orine , (NC State) DEC Haiden Drury , (Utah Valley), 3-2</t>
         </is>
       </c>
     </row>
@@ -4468,7 +4468,7 @@
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>Devan Turner , (Oregon State) DEC Sidney Flores , (Air Force), 9-2</t>
+          <t>Matt Ramos , (Purdue) DEC Rayvon Foley , (Michigan State), 9-6</t>
         </is>
       </c>
     </row>
@@ -4480,7 +4480,7 @@
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>Chance Rich , (Cal State Bakersfield) DEC Kyle Biscoglia , (Northern Iowa), 3-1</t>
+          <t>Devan Turner , (Oregon State) DEC Sidney Flores , (Air Force), 9-2</t>
         </is>
       </c>
     </row>
@@ -4492,7 +4492,7 @@
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>Richie Koehler , (Rider) FOR Brock Hudkins , (Indiana)</t>
+          <t>Chance Rich , (Cal State Bakersfield) DEC Kyle Biscoglia , (Northern Iowa), 3-1</t>
         </is>
       </c>
     </row>
@@ -4504,7 +4504,7 @@
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>Micky Phillippi , (Pittsburgh) DEC Joe Olivieri , (Rutgers), 4-2</t>
+          <t>Richie Koehler , (Rider) FOR Brock Hudkins , (Indiana)</t>
         </is>
       </c>
     </row>
@@ -4516,7 +4516,7 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>Lucas Byrd , (Illinois) DEC Michael Colaiocco , (Penn), 7-5 SV</t>
+          <t>Micky Phillippi , (Pittsburgh) DEC Joe Olivieri , (Rutgers), 4-2</t>
         </is>
       </c>
     </row>
@@ -4528,19 +4528,19 @@
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>Joseph Heilmann , (North Carolina) DEC Joshua Koderhandt , (Navy), 6-0</t>
+          <t>Lucas Byrd , (Illinois) DEC Michael Colaiocco , (Penn), 7-5 SV</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>133</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>Jaydin Eierman , (Iowa) DEC Dylan D`emilio , (Ohio State), 5-3</t>
+          <t>Joseph Heilmann , (North Carolina) DEC Joshua Koderhandt , (Navy), 6-0</t>
         </is>
       </c>
     </row>
@@ -4552,7 +4552,7 @@
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>Stevan Micic , (Michigan) MD Frankie Tal sharar , (Northwestern), 10-2</t>
+          <t>Jaydin Eierman , (Iowa) DEC Dylan D`emilio , (Ohio State), 5-3</t>
         </is>
       </c>
     </row>
@@ -4564,7 +4564,7 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>Dylan Droegemueller , (North Dakota State) DEC Matt Kazimir , (Columbia), 6-1</t>
+          <t>Stevan Micic , (Michigan) MD Frankie Tal sharar , (Northwestern), 10-2</t>
         </is>
       </c>
     </row>
@@ -4576,7 +4576,7 @@
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>Chad Red , (Nebraska) DEC Ian Parker , (Iowa State), 7-5</t>
+          <t>Dylan Droegemueller , (North Dakota State) DEC Matt Kazimir , (Columbia), 6-1</t>
         </is>
       </c>
     </row>
@@ -4588,7 +4588,7 @@
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>Dresden Simon , (Central Michigan) DEC Parker Filius , (Purdue), 8-7</t>
+          <t>Chad Red , (Nebraska) DEC Ian Parker , (Iowa State), 7-5</t>
         </is>
       </c>
     </row>
@@ -4600,7 +4600,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>Andrew Alirez , (Northern Colorado) MD Joseph Zargo , (Wisconsin), 8-0</t>
+          <t>Dresden Simon , (Central Michigan) DEC Parker Filius , (Purdue), 8-7</t>
         </is>
       </c>
     </row>
@@ -4612,7 +4612,7 @@
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>Clay Carlson , (South Dakota State) DEC Allan Hart , (Missouri), 7-5 SV</t>
+          <t>Andrew Alirez , (Northern Colorado) MD Joseph Zargo , (Wisconsin), 8-0</t>
         </is>
       </c>
     </row>
@@ -4624,19 +4624,19 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>Ryan Jack , (NC State) DEC Quinn Kinner , (Rider), 6-4</t>
+          <t>Clay Carlson , (South Dakota State) DEC Allan Hart , (Missouri), 7-5 SV</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>141</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>Anthony Artalona , (Penn) DEC Zachary Sherman , (North Carolina), 8-4</t>
+          <t>Ryan Jack , (NC State) DEC Quinn Kinner , (Rider), 6-4</t>
         </is>
       </c>
     </row>
@@ -4648,7 +4648,7 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>Pj Ogunsanya , (Army) F Joshua Heil , (Campbell), 6:56</t>
+          <t>Anthony Artalona , (Penn) DEC Zachary Sherman , (North Carolina), 8-4</t>
         </is>
       </c>
     </row>
@@ -4660,7 +4660,7 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>Jonathan Millner , (Appalachian State) DEC Mike Van brill , (Rutgers), 5-1</t>
+          <t>Pj Ogunsanya , (Army) F Joshua Heil , (Campbell), 6:56</t>
         </is>
       </c>
     </row>
@@ -4672,7 +4672,7 @@
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>Colin Realbuto , (Northern Iowa) DEC Josh Finesilver , (Duke), 8-4</t>
+          <t>Jonathan Millner , (Appalachian State) DEC Mike Van brill , (Rutgers), 5-1</t>
         </is>
       </c>
     </row>
@@ -4684,7 +4684,7 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>Yahya Thomas , (Northwestern) DEC Beau Bartlett , (Penn State), 5-3</t>
+          <t>Colin Realbuto , (Northern Iowa) DEC Josh Finesilver , (Duke), 8-4</t>
         </is>
       </c>
     </row>
@@ -4696,7 +4696,7 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>Cory Crooks , (Oregon State) DEC Marcus Robinson , (Cleveland State), 5-3 SV</t>
+          <t>Yahya Thomas , (Northwestern) DEC Beau Bartlett , (Penn State), 5-3</t>
         </is>
       </c>
     </row>
@@ -4708,7 +4708,7 @@
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>Kaden Gfeller , (Oklahoma State) F Jaden Abas , (Stanford), 2:49</t>
+          <t>Cory Crooks , (Oregon State) DEC Marcus Robinson , (Cleveland State), 5-3 SV</t>
         </is>
       </c>
     </row>
@@ -4720,19 +4720,19 @@
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>Willie Mcdougald , (Oklahoma) F Michael Blockhus , (Minnesota), 8:57</t>
+          <t>Kaden Gfeller , (Oklahoma State) F Jaden Abas , (Stanford), 2:49</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>149</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>Brady Berge , (Penn State) DEC Johnny Lovett , (Central Michigan), 4-3</t>
+          <t>Willie Mcdougald , (Oklahoma) F Michael Blockhus , (Minnesota), 8:57</t>
         </is>
       </c>
     </row>
@@ -4744,7 +4744,7 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>Peyton Robb , (Nebraska) DEC Doug Zapf , (Penn), 3-2</t>
+          <t>Brady Berge , (Penn State) DEC Johnny Lovett , (Central Michigan), 4-3</t>
         </is>
       </c>
     </row>
@@ -4756,7 +4756,7 @@
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>Dazjon Casto , (The Citadel) DEC Connor Brady , (Virginia Tech), 3-1 SV</t>
+          <t>Peyton Robb , (Nebraska) DEC Doug Zapf , (Penn), 3-2</t>
         </is>
       </c>
     </row>
@@ -4768,7 +4768,7 @@
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>Jake Keating , (Virginia) DEC Elijah Cleary , (Pittsburgh), 3-2</t>
+          <t>Dazjon Casto , (The Citadel) DEC Connor Brady , (Virginia Tech), 3-1 SV</t>
         </is>
       </c>
     </row>
@@ -4780,7 +4780,7 @@
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>Hunter Richard , (Cornell) DEC Justin Thomas , (Oklahoma), 6-5</t>
+          <t>Jake Keating , (Virginia) DEC Elijah Cleary , (Pittsburgh), 3-2</t>
         </is>
       </c>
     </row>
@@ -4792,7 +4792,7 @@
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>Austin O`connor , (North Carolina) DEC Jacob Wright , (Wyoming), 4-2</t>
+          <t>Hunter Richard , (Cornell) DEC Justin Thomas , (Oklahoma), 6-5</t>
         </is>
       </c>
     </row>
@@ -4804,7 +4804,7 @@
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>Kaleb Young , (Iowa) MD Markus Hartman , (Army), 9-1</t>
+          <t>Austin O`connor , (North Carolina) DEC Jacob Wright , (Wyoming), 4-2</t>
         </is>
       </c>
     </row>
@@ -4816,19 +4816,19 @@
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>David Carr , (Iowa State) DEC Wyatt Sheets , (Oklahoma State), 3-2</t>
+          <t>Kaleb Young , (Iowa) MD Markus Hartman , (Army), 9-1</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>157</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>Anthony Valencia , (Arizona State) DEC Matthew Olguin , (Oregon State), 3-1 SV</t>
+          <t>David Carr , (Iowa State) DEC Wyatt Sheets , (Oklahoma State), 3-2</t>
         </is>
       </c>
     </row>
@@ -4840,7 +4840,7 @@
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>Jake Wentzel , (Pittsburgh) DEC Brevin Cassella , (Binghamton), 2-0</t>
+          <t>Anthony Valencia , (Arizona State) DEC Matthew Olguin , (Oregon State), 3-1 SV</t>
         </is>
       </c>
     </row>
@@ -4852,7 +4852,7 @@
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>Izzak Olejnik , (Northern Illinois) DEC Thomas Bullard , (NC State), 4-2</t>
+          <t>Jake Wentzel , (Pittsburgh) DEC Brevin Cassella , (Binghamton), 2-0</t>
         </is>
       </c>
     </row>
@@ -4864,7 +4864,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>Justin Mccoy , (Virginia) MD William Formato , (Appalachian State), 14-4</t>
+          <t>Izzak Olejnik , (Northern Illinois) DEC Thomas Bullard , (NC State), 4-2</t>
         </is>
       </c>
     </row>
@@ -4876,7 +4876,7 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>Julian Ramirez , (Cornell) MD Joshua Ogunsanya , (Columbia), 14-3</t>
+          <t>Justin Mccoy , (Virginia) MD William Formato , (Appalachian State), 14-4</t>
         </is>
       </c>
     </row>
@@ -4888,7 +4888,7 @@
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>Zach Hartman , (Bucknell) MD Clayton Wilson , (Nebraska), 13-3</t>
+          <t>Julian Ramirez , (Cornell) MD Joshua Ogunsanya , (Columbia), 14-3</t>
         </is>
       </c>
     </row>
@@ -4900,7 +4900,7 @@
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>Philip Conigliaro , (Harvard) DEC Lucas Revano , (Penn), 5-3</t>
+          <t>Zach Hartman , (Bucknell) MD Clayton Wilson , (Nebraska), 13-3</t>
         </is>
       </c>
     </row>
@@ -4912,19 +4912,19 @@
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>Austin Yant , (Northern Iowa) DEC Luke Weber , (North Dakota State), 3-2</t>
+          <t>Philip Conigliaro , (Harvard) DEC Lucas Revano , (Penn), 5-3</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>174</t>
+          <t>165</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>Lance Runyon , (Northern Iowa) DEC Nick Incontrera , (Penn), 8-2</t>
+          <t>Austin Yant , (Northern Iowa) DEC Luke Weber , (North Dakota State), 3-2</t>
         </is>
       </c>
     </row>
@@ -4936,7 +4936,7 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>Michael O'malley Hasbrouck Heights, NJ (Drexel) F Tyler Eischens , (Stanford), 2:46</t>
+          <t>Lance Runyon , (Northern Iowa) DEC Nick Incontrera , (Penn), 8-2</t>
         </is>
       </c>
     </row>
@@ -4948,7 +4948,7 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>Mason Kauffman , (Northern Illinois) DEC Benjamin Pasiuk , (Army), 3-2</t>
+          <t>Michael O'malley Hasbrouck Heights, NJ (Drexel) F Tyler Eischens , (Stanford), 2:46</t>
         </is>
       </c>
     </row>
@@ -4960,7 +4960,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>Hayden Hastings , (Wyoming) F Thomas Flitz , (Appalachian State), 2:21</t>
+          <t>Mason Kauffman , (Northern Illinois) DEC Benjamin Pasiuk , (Army), 3-2</t>
         </is>
       </c>
     </row>
@@ -4972,7 +4972,7 @@
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>Matthew Finesilver , (Duke) DEC Christopher Foca , (Cornell), 8-2</t>
+          <t>Hayden Hastings , (Wyoming) F Thomas Flitz , (Appalachian State), 2:21</t>
         </is>
       </c>
     </row>
@@ -4984,7 +4984,7 @@
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>Peyton Mocco , (Missouri) DEC Cade Devos , (South Dakota State), 6-2</t>
+          <t>Matthew Finesilver , (Duke) DEC Christopher Foca , (Cornell), 8-2</t>
         </is>
       </c>
     </row>
@@ -4996,7 +4996,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>Ethan Smith , (Ohio State) F Gerrit Nijenhuis , (Purdue), 6:59</t>
+          <t>Peyton Mocco , (Missouri) DEC Cade Devos , (South Dakota State), 6-2</t>
         </is>
       </c>
     </row>
@@ -5008,19 +5008,19 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>Anthony Mantanona , (Oklahoma) DEC Adam Kemp , (California Poly), 4-1</t>
+          <t>Ethan Smith , (Ohio State) F Gerrit Nijenhuis , (Purdue), 6:59</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>184</t>
+          <t>174</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>Jeremiah Kent , (Missouri) DEC Hunter Bolen , (Virginia Tech), 4-2</t>
+          <t>Anthony Mantanona , (Oklahoma) DEC Adam Kemp , (California Poly), 4-1</t>
         </is>
       </c>
     </row>
@@ -5032,7 +5032,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>Taylor Venz , (Nebraska) MD Caleb Hopkins , (Campbell), 10-0</t>
+          <t>Jeremiah Kent , (Missouri) DEC Hunter Bolen , (Virginia Tech), 4-2</t>
         </is>
       </c>
     </row>
@@ -5044,7 +5044,7 @@
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>Jonathan Loew , (Cornell) DEC Brit Wilson , (Northern Illinois), 11-4</t>
+          <t>Taylor Venz , (Nebraska) MD Caleb Hopkins , (Campbell), 10-0</t>
         </is>
       </c>
     </row>
@@ -5056,7 +5056,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>John Poznanski , (Rutgers) DEC Isaiah Salazar , (Minnesota), 10-7</t>
+          <t>Jonathan Loew , (Cornell) DEC Brit Wilson , (Northern Illinois), 11-4</t>
         </is>
       </c>
     </row>
@@ -5068,7 +5068,7 @@
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>Max Lyon , (Purdue) DEC Kyle Cochran , (Maryland), 6-4 SV</t>
+          <t>John Poznanski , (Rutgers) DEC Isaiah Salazar , (Minnesota), 10-7</t>
         </is>
       </c>
     </row>
@@ -5080,7 +5080,7 @@
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>Keegan Moore , (Oklahoma) DEC Tate Samuelson , (Wyoming), 6-3</t>
+          <t>Max Lyon , (Purdue) DEC Kyle Cochran , (Maryland), 6-4 SV</t>
         </is>
       </c>
     </row>
@@ -5092,7 +5092,7 @@
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>Marcus Coleman , (Iowa State) DEC Travis Stefanik , (Princeton), 6-1</t>
+          <t>Keegan Moore , (Oklahoma) DEC Tate Samuelson , (Wyoming), 6-3</t>
         </is>
       </c>
     </row>
@@ -5104,19 +5104,19 @@
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>Dakota Geer , (Oklahoma State) DEC Abe Assad , (Iowa), 5-3 SV</t>
+          <t>Marcus Coleman , (Iowa State) DEC Travis Stefanik , (Princeton), 6-1</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>197</t>
+          <t>184</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>Kordell Norfleet , (Arizona State) DEF Luke Stout , (Princeton)</t>
+          <t>Dakota Geer , (Oklahoma State) DEC Abe Assad , (Iowa), 5-3 SV</t>
         </is>
       </c>
     </row>
@@ -5128,7 +5128,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>Yonger Bastida , (Iowa State) DEC Jaron Smith , (Maryland), 11-4</t>
+          <t>Kordell Norfleet , (Arizona State) DEF Luke Stout , (Princeton)</t>
         </is>
       </c>
     </row>
@@ -5140,7 +5140,7 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>Thomas Penola , (Purdue) DEC Tanner Sloan , (South Dakota State), 10-8 SV</t>
+          <t>Yonger Bastida , (Iowa State) DEC Jaron Smith , (Maryland), 11-4</t>
         </is>
       </c>
     </row>
@@ -5152,7 +5152,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>Greg Bulsak , (Rutgers) MD Jacob Koser , (Navy), 8-0</t>
+          <t>Thomas Penola , (Purdue) DEC Tanner Sloan , (South Dakota State), 10-8 SV</t>
         </is>
       </c>
     </row>
@@ -5164,7 +5164,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>Patrick Brucki , (Michigan) DEC Jacob Cardenas , (Cornell), 8-6 SV</t>
+          <t>Greg Bulsak , (Rutgers) MD Jacob Koser , (Navy), 8-0</t>
         </is>
       </c>
     </row>
@@ -5176,7 +5176,7 @@
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>Nino Bonaccorsi , (Pittsburgh) DEC Owen Pentz , (North Dakota State), 3-2</t>
+          <t>Patrick Brucki , (Michigan) DEC Jacob Cardenas , (Cornell), 8-6 SV</t>
         </is>
       </c>
     </row>
@@ -5188,7 +5188,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>Cameron Caffey , (Michigan State) DEC Braxton Amos , (Wisconsin), 6-5</t>
+          <t>Nino Bonaccorsi , (Pittsburgh) DEC Owen Pentz , (North Dakota State), 3-2</t>
         </is>
       </c>
     </row>
@@ -5200,19 +5200,19 @@
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>Jay Aiello , (Virginia) DEC Isaac Trumble , (NC State), 6-5</t>
+          <t>Cameron Caffey , (Michigan State) DEC Braxton Amos , (Wisconsin), 6-5</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>285</t>
+          <t>197</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>Lewis Fernandes , (Cornell) DEC Trent Hillger , (Wisconsin), 2-1</t>
+          <t>Jay Aiello , (Virginia) DEC Isaac Trumble , (NC State), 6-5</t>
         </is>
       </c>
     </row>
@@ -5224,7 +5224,7 @@
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>Nathan Traxler , (Virginia Tech) DEC Isaac Reid , (Lock Haven), 6-5</t>
+          <t>Lewis Fernandes , (Cornell) DEC Trent Hillger , (Wisconsin), 2-1</t>
         </is>
       </c>
     </row>
@@ -5236,7 +5236,7 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>Gary Traub , (Oregon State) DEC Tyrie Houghton , (NC State), 5-1 SV</t>
+          <t>Nathan Traxler , (Virginia Tech) DEC Isaac Reid , (Lock Haven), 6-5</t>
         </is>
       </c>
     </row>
@@ -5248,7 +5248,7 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>Joe Doyle , (Binghamton) MD Luke Luffman , (Illinois), 14-4</t>
+          <t>Gary Traub , (Oregon State) DEC Tyrie Houghton , (NC State), 5-1 SV</t>
         </is>
       </c>
     </row>
@@ -5260,7 +5260,7 @@
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>Tate Orndorff , (Ohio State) DEC Luke Surber , (Oklahoma State), 5-0</t>
+          <t>Joe Doyle , (Binghamton) MD Luke Luffman , (Illinois), 14-4</t>
         </is>
       </c>
     </row>
@@ -5272,7 +5272,7 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>Wyatt Hendrickson , (Air Force) MD Aj Nevills , (South Dakota State), 13-1</t>
+          <t>Tate Orndorff , (Ohio State) DEC Luke Surber , (Oklahoma State), 5-0</t>
         </is>
       </c>
     </row>
@@ -5284,7 +5284,7 @@
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>Matt Stencel , (Central Michigan) DEC Ben Goldin , (Penn), 4-2</t>
+          <t>Wyatt Hendrickson , (Air Force) MD Aj Nevills , (South Dakota State), 13-1</t>
         </is>
       </c>
     </row>
@@ -5296,26 +5296,26 @@
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>Zach Elam , (Missouri) F Taye Ghadiali , (Campbell), 5:58</t>
+          <t>Matt Stencel , (Central Michigan) DEC Ben Goldin , (Penn), 4-2</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>CONSI OF 16 #1</t>
+          <t>285</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Zach Elam , (Missouri) F Taye Ghadiali , (Campbell), 5:58</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>125</t>
-        </is>
-      </c>
-      <c r="B414" t="inlineStr">
-        <is>
-          <t>Drew Hildebrandt , (Penn State) DEC Logan Ashton , (Stanford), 3-1</t>
+          <t>CONSI OF 16 #1</t>
         </is>
       </c>
     </row>
@@ -5327,7 +5327,7 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>Patrick Mckee , (Minnesota) MD Devin Schroder , (Purdue), 11-0</t>
+          <t>Drew Hildebrandt , (Penn State) DEC Logan Ashton , (Stanford), 3-1</t>
         </is>
       </c>
     </row>
@@ -5339,7 +5339,7 @@
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>Malik Heinselman , (Ohio State) DEC Korbin Meink , (Campbell), 10-4</t>
+          <t>Patrick Mckee , (Minnesota) MD Devin Schroder , (Purdue), 11-0</t>
         </is>
       </c>
     </row>
@@ -5351,7 +5351,7 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>Drake Ayala , (Iowa) DEC Joe Manchio , (Columbia), 7-1</t>
+          <t>Malik Heinselman , (Ohio State) DEC Korbin Meink , (Campbell), 10-4</t>
         </is>
       </c>
     </row>
@@ -5363,7 +5363,7 @@
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>Joey Prata , (Oklahoma) DEC Jace Koelzer , (Northern Colorado), 4-1</t>
+          <t>Drake Ayala , (Iowa) DEC Joe Manchio , (Columbia), 7-1</t>
         </is>
       </c>
     </row>
@@ -5375,7 +5375,7 @@
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>Ryan Miller , (Penn) DEC Justin Cardani , (Illinois), 5-1</t>
+          <t>Joey Prata , (Oklahoma) DEC Jace Koelzer , (Northern Colorado), 4-1</t>
         </is>
       </c>
     </row>
@@ -5387,7 +5387,7 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>Dylan Shawver , (Rutgers) DEC Kysen Terukina , (Iowa State), 6-4</t>
+          <t>Ryan Miller , (Penn) DEC Justin Cardani , (Illinois), 5-1</t>
         </is>
       </c>
     </row>
@@ -5399,19 +5399,19 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>Noah Surtin , (Missouri) DEC Antonio Lorenzo , (California Poly), 2-1</t>
+          <t>Dylan Shawver , (Rutgers) DEC Kysen Terukina , (Iowa State), 6-4</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>125</t>
         </is>
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>Haiden Drury , (Utah Valley) DEC Dominic Lajoie , (Cornell), 10-5</t>
+          <t>Noah Surtin , (Missouri) DEC Antonio Lorenzo , (California Poly), 2-1</t>
         </is>
       </c>
     </row>
@@ -5423,7 +5423,7 @@
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>Rayvon Foley , (Michigan State) M FOR Ramazan Attasauov , (Iowa State)</t>
+          <t>Haiden Drury , (Utah Valley) DEC Dominic Lajoie , (Cornell), 10-5</t>
         </is>
       </c>
     </row>
@@ -5435,7 +5435,7 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>Sidney Flores , (Air Force) DEC Codi Russell , (Appalachian State), 12-9</t>
+          <t>Rayvon Foley , (Michigan State) M FOR Ramazan Attasauov , (Iowa State)</t>
         </is>
       </c>
     </row>
@@ -5447,7 +5447,7 @@
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>Chance Rich , (Cal State Bakersfield) DEC Jake Gliva , (Minnesota), 12-9</t>
+          <t>Sidney Flores , (Air Force) DEC Codi Russell , (Appalachian State), 12-9</t>
         </is>
       </c>
     </row>
@@ -5459,7 +5459,7 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>Richie Koehler , (Rider) DEC Brayden Palmer , (Chattanooga), 4-2</t>
+          <t>Chance Rich , (Cal State Bakersfield) DEC Jake Gliva , (Minnesota), 12-9</t>
         </is>
       </c>
     </row>
@@ -5471,7 +5471,7 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>Joe Olivieri , (Rutgers) DEC Malyke Hines , (Lehigh), 7-3</t>
+          <t>Richie Koehler , (Rider) DEC Brayden Palmer , (Chattanooga), 4-2</t>
         </is>
       </c>
     </row>
@@ -5483,7 +5483,7 @@
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>Lucas Byrd , (Illinois) DEC Anthony Madrigal , (Oklahoma), 3-1</t>
+          <t>Joe Olivieri , (Rutgers) DEC Malyke Hines , (Lehigh), 7-3</t>
         </is>
       </c>
     </row>
@@ -5495,19 +5495,19 @@
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>Joseph Heilmann , (North Carolina) DEC Kyle Burwick , (Wisconsin), 6-2</t>
+          <t>Lucas Byrd , (Illinois) DEC Anthony Madrigal , (Oklahoma), 3-1</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>133</t>
         </is>
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>Dylan D`emilio , (Ohio State) DEC Josh Mason , (Bloomsburg), 9-6</t>
+          <t>Joseph Heilmann , (North Carolina) DEC Kyle Burwick , (Wisconsin), 6-2</t>
         </is>
       </c>
     </row>
@@ -5519,7 +5519,7 @@
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>Stevan Micic , (Michigan) DEC Carter Young , (Oklahoma State), 7-4</t>
+          <t>Dylan D`emilio , (Ohio State) DEC Josh Mason , (Bloomsburg), 9-6</t>
         </is>
       </c>
     </row>
@@ -5531,7 +5531,7 @@
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>Dylan Droegemueller , (North Dakota State) DEC Collin Gerardi , (Virginia Tech), 7-1</t>
+          <t>Stevan Micic , (Michigan) DEC Carter Young , (Oklahoma State), 7-4</t>
         </is>
       </c>
     </row>
@@ -5543,7 +5543,7 @@
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>Ian Parker , (Iowa State) DEC Connor Mcgonagle , (Lehigh), 6-1</t>
+          <t>Dylan Droegemueller , (North Dakota State) DEC Collin Gerardi , (Virginia Tech), 7-1</t>
         </is>
       </c>
     </row>
@@ -5555,7 +5555,7 @@
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>Dresden Simon , (Central Michigan) MD Jacob Butler , (Oklahoma), 14-5</t>
+          <t>Ian Parker , (Iowa State) DEC Connor Mcgonagle , (Lehigh), 6-1</t>
         </is>
       </c>
     </row>
@@ -5567,7 +5567,7 @@
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>Joseph Zargo , (Wisconsin) DEC Shannon Hanna , (Campbell), 9-8</t>
+          <t>Dresden Simon , (Central Michigan) MD Jacob Butler , (Oklahoma), 14-5</t>
         </is>
       </c>
     </row>
@@ -5579,7 +5579,7 @@
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>Clay Carlson , (South Dakota State) DEC Gabe Willochell , (Edinboro), 10-5</t>
+          <t>Joseph Zargo , (Wisconsin) DEC Shannon Hanna , (Campbell), 9-8</t>
         </is>
       </c>
     </row>
@@ -5591,19 +5591,19 @@
       </c>
       <c r="B437" t="inlineStr">
         <is>
-          <t>Ryan Jack , (NC State) DEC Wilfredo Gil , (Franklin &amp; Marshall), 10-5</t>
+          <t>Clay Carlson , (South Dakota State) DEC Gabe Willochell , (Edinboro), 10-5</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>141</t>
         </is>
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>Zachary Sherman , (North Carolina) DEC Jarrett Degen , (Iowa State), 5-2</t>
+          <t>Ryan Jack , (NC State) DEC Wilfredo Gil , (Franklin &amp; Marshall), 10-5</t>
         </is>
       </c>
     </row>
@@ -5615,7 +5615,7 @@
       </c>
       <c r="B439" t="inlineStr">
         <is>
-          <t>Pj Ogunsanya , (Army) DEC Corbyn Munson , (Central Michigan), 12-7</t>
+          <t>Zachary Sherman , (North Carolina) DEC Jarrett Degen , (Iowa State), 5-2</t>
         </is>
       </c>
     </row>
@@ -5627,7 +5627,7 @@
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>Mike Van brill , (Rutgers) DEC Kody Komara , (Kent State), 4-0</t>
+          <t>Pj Ogunsanya , (Army) DEC Corbyn Munson , (Central Michigan), 12-7</t>
         </is>
       </c>
     </row>
@@ -5639,7 +5639,7 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>Colin Realbuto , (Northern Iowa) F John Arceri , (Buffalo), 2:16</t>
+          <t>Mike Van brill , (Rutgers) DEC Kody Komara , (Kent State), 4-0</t>
         </is>
       </c>
     </row>
@@ -5651,7 +5651,7 @@
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>Yahya Thomas , (Northwestern) F Marshall Keller , (Princeton), 4:24</t>
+          <t>Colin Realbuto , (Northern Iowa) F John Arceri , (Buffalo), 2:16</t>
         </is>
       </c>
     </row>
@@ -5663,7 +5663,7 @@
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>Cory Crooks , (Oregon State) DEC Max Brignola , (Lehigh), 7-6</t>
+          <t>Yahya Thomas , (Northwestern) F Marshall Keller , (Princeton), 4:24</t>
         </is>
       </c>
     </row>
@@ -5675,7 +5675,7 @@
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>Jaden Abas , (Stanford) DEC Joshua Edmond , (Missouri), 9-3</t>
+          <t>Cory Crooks , (Oregon State) DEC Max Brignola , (Lehigh), 7-6</t>
         </is>
       </c>
     </row>
@@ -5687,19 +5687,19 @@
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>Michael Blockhus , (Minnesota) DEC Legend Lamer , (California Poly), 5-1</t>
+          <t>Jaden Abas , (Stanford) DEC Joshua Edmond , (Missouri), 9-3</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>149</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>Brady Berge , (Penn State) MD Derek Holschlag , (Northern Iowa), 15-7</t>
+          <t>Michael Blockhus , (Minnesota) DEC Legend Lamer , (California Poly), 5-1</t>
         </is>
       </c>
     </row>
@@ -5711,7 +5711,7 @@
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t>Doug Zapf , (Penn) DEC Jarrett Jacques , (Missouri), 2-1</t>
+          <t>Brady Berge , (Penn State) MD Derek Holschlag , (Northern Iowa), 15-7</t>
         </is>
       </c>
     </row>
@@ -5723,7 +5723,7 @@
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t>Connor Brady , (Virginia Tech) DEC Chase Saldate , (Michigan State), 3-2</t>
+          <t>Doug Zapf , (Penn) DEC Jarrett Jacques , (Missouri), 2-1</t>
         </is>
       </c>
     </row>
@@ -5735,7 +5735,7 @@
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t>Elijah Cleary , (Pittsburgh) DEC Michael Petite , (Buffalo), 3-2</t>
+          <t>Connor Brady , (Virginia Tech) DEC Chase Saldate , (Michigan State), 3-2</t>
         </is>
       </c>
     </row>
@@ -5747,7 +5747,7 @@
       </c>
       <c r="B450" t="inlineStr">
         <is>
-          <t>Hunter Richard , (Cornell) DEC Kendall Coleman , (Purdue), 3-2</t>
+          <t>Elijah Cleary , (Pittsburgh) DEC Michael Petite , (Buffalo), 3-2</t>
         </is>
       </c>
     </row>
@@ -5759,7 +5759,7 @@
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>Austin O`connor , (North Carolina) DEC Garrett Model , (Wisconsin), 5-2</t>
+          <t>Hunter Richard , (Cornell) DEC Kendall Coleman , (Purdue), 3-2</t>
         </is>
       </c>
     </row>
@@ -5771,7 +5771,7 @@
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>Markus Hartman , (Army) DEC Ben Barton , (Lock Haven), 9-6</t>
+          <t>Austin O`connor , (North Carolina) DEC Garrett Model , (Wisconsin), 5-2</t>
         </is>
       </c>
     </row>
@@ -5783,19 +5783,19 @@
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>Wyatt Sheets , (Oklahoma State) DEC Andrew Cerniglia , (Navy), 9-5</t>
+          <t>Markus Hartman , (Army) DEC Ben Barton , (Lock Haven), 9-6</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>157</t>
         </is>
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>Matthew Olguin , (Oregon State) DEC Brian Meyer , (Lehigh), 2-1</t>
+          <t>Wyatt Sheets , (Oklahoma State) DEC Andrew Cerniglia , (Navy), 9-5</t>
         </is>
       </c>
     </row>
@@ -5807,7 +5807,7 @@
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>Brevin Cassella , (Binghamton) DEC Riley Smucker , (Cleveland State), 7-0</t>
+          <t>Matthew Olguin , (Oregon State) DEC Brian Meyer , (Lehigh), 2-1</t>
         </is>
       </c>
     </row>
@@ -5819,7 +5819,7 @@
       </c>
       <c r="B456" t="inlineStr">
         <is>
-          <t>Thomas Bullard , (NC State) TF Cael Carlson , (Minnesota), 15-0 3:17</t>
+          <t>Brevin Cassella , (Binghamton) DEC Riley Smucker , (Cleveland State), 7-0</t>
         </is>
       </c>
     </row>
@@ -5831,7 +5831,7 @@
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>William Formato , (Appalachian State) M FOR Andrew Nicholson , (Chattanooga)</t>
+          <t>Thomas Bullard , (NC State) TF Cael Carlson , (Minnesota), 15-0 3:17</t>
         </is>
       </c>
     </row>
@@ -5843,7 +5843,7 @@
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>Joshua Ogunsanya , (Columbia) DEC Evan Barczak , (Drexel), 3-1</t>
+          <t>William Formato , (Appalachian State) M FOR Andrew Nicholson , (Chattanooga)</t>
         </is>
       </c>
     </row>
@@ -5855,7 +5855,7 @@
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>Clayton Wilson , (Nebraska) DEC Rodrick Mosley , (Gardner-Webb), 3-1</t>
+          <t>Joshua Ogunsanya , (Columbia) DEC Evan Barczak , (Drexel), 3-1</t>
         </is>
       </c>
     </row>
@@ -5867,7 +5867,7 @@
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>Lucas Revano , (Penn) DEC Ashton Eyler , (Lock Haven), 6-3</t>
+          <t>Clayton Wilson , (Nebraska) DEC Rodrick Mosley , (Gardner-Webb), 3-1</t>
         </is>
       </c>
     </row>
@@ -5879,19 +5879,19 @@
       </c>
       <c r="B461" t="inlineStr">
         <is>
-          <t>Austin Yant , (Northern Iowa) DEC Caleb Fish , (Michigan State), 6-2</t>
+          <t>Lucas Revano , (Penn) DEC Ashton Eyler , (Lock Haven), 6-3</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>174</t>
+          <t>165</t>
         </is>
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>Nick Incontrera , (Penn) F Connor Oneill , (Rutgers), 1:54</t>
+          <t>Austin Yant , (Northern Iowa) DEC Caleb Fish , (Michigan State), 6-2</t>
         </is>
       </c>
     </row>
@@ -5903,7 +5903,7 @@
       </c>
       <c r="B463" t="inlineStr">
         <is>
-          <t>Michael O'malley Hasbrouck Heights, NJ (Drexel) DEC Joel Devine , (Iowa State), 4-1</t>
+          <t>Nick Incontrera , (Penn) F Connor Oneill , (Rutgers), 1:54</t>
         </is>
       </c>
     </row>
@@ -5915,7 +5915,7 @@
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>Benjamin Pasiuk , (Army) DEC Bailee O`reilly , (Minnesota), 7-1</t>
+          <t>Michael O'malley Hasbrouck Heights, NJ (Drexel) DEC Joel Devine , (Iowa State), 4-1</t>
         </is>
       </c>
     </row>
@@ -5927,7 +5927,7 @@
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>Hayden Hastings , (Wyoming) MD Jay Nivison Buffalo, NY (Buffalo), 8-0</t>
+          <t>Benjamin Pasiuk , (Army) DEC Bailee O`reilly , (Minnesota), 7-1</t>
         </is>
       </c>
     </row>
@@ -5939,7 +5939,7 @@
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>Christopher Foca , (Cornell) F Jacob Nolan , (Binghamton), 5:17</t>
+          <t>Hayden Hastings , (Wyoming) MD Jay Nivison Buffalo, NY (Buffalo), 8-0</t>
         </is>
       </c>
     </row>
@@ -5951,7 +5951,7 @@
       </c>
       <c r="B467" t="inlineStr">
         <is>
-          <t>Peyton Mocco , (Missouri) MD Sal Perrine , (Ohio), 15-6</t>
+          <t>Christopher Foca , (Cornell) F Jacob Nolan , (Binghamton), 5:17</t>
         </is>
       </c>
     </row>
@@ -5963,7 +5963,7 @@
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>Ethan Smith , (Ohio State) MD Troy Fisher , (Northwestern), 14-5</t>
+          <t>Peyton Mocco , (Missouri) MD Sal Perrine , (Ohio), 15-6</t>
         </is>
       </c>
     </row>
@@ -5975,19 +5975,19 @@
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>Anthony Mantanona , (Oklahoma) DEC Dennis Robin , (West Virginia), 5-3</t>
+          <t>Ethan Smith , (Ohio State) MD Troy Fisher , (Northwestern), 14-5</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>184</t>
+          <t>174</t>
         </is>
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>Jeremiah Kent , (Missouri) F Colin Mccracken , (Kent State), 0:42</t>
+          <t>Anthony Mantanona , (Oklahoma) DEC Dennis Robin , (West Virginia), 5-3</t>
         </is>
       </c>
     </row>
@@ -5999,7 +5999,7 @@
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>Caleb Hopkins , (Campbell) F Michael Battista , (Virginia), 1:42</t>
+          <t>Jeremiah Kent , (Missouri) F Colin Mccracken , (Kent State), 0:42</t>
         </is>
       </c>
     </row>
@@ -6011,7 +6011,7 @@
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>Brit Wilson , (Northern Illinois) MD Gregg Harvey , (Pittsburgh), 17-3</t>
+          <t>Caleb Hopkins , (Campbell) F Michael Battista , (Virginia), 1:42</t>
         </is>
       </c>
     </row>
@@ -6023,7 +6023,7 @@
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>John Poznanski , (Rutgers) DEC Christopher Weiler , (Wisconsin), 6-1</t>
+          <t>Brit Wilson , (Northern Illinois) MD Gregg Harvey , (Pittsburgh), 17-3</t>
         </is>
       </c>
     </row>
@@ -6035,7 +6035,7 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>Max Lyon , (Purdue) DEC Gavin Kane , (North Carolina), 6-4</t>
+          <t>John Poznanski , (Rutgers) DEC Christopher Weiler , (Wisconsin), 6-1</t>
         </is>
       </c>
     </row>
@@ -6047,7 +6047,7 @@
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>Keegan Moore , (Oklahoma) DEC Layne Malczewski , (Michigan State), 11-5</t>
+          <t>Max Lyon , (Purdue) DEC Gavin Kane , (North Carolina), 6-4</t>
         </is>
       </c>
     </row>
@@ -6059,7 +6059,7 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>Travis Stefanik , (Princeton) DEC Donnell Washington , (Indiana), 6-1</t>
+          <t>Keegan Moore , (Oklahoma) DEC Layne Malczewski , (Michigan State), 11-5</t>
         </is>
       </c>
     </row>
@@ -6071,19 +6071,19 @@
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>Abe Assad , (Iowa) DEC Aj Burkhart , (Lehigh), 9-3</t>
+          <t>Travis Stefanik , (Princeton) DEC Donnell Washington , (Indiana), 6-1</t>
         </is>
       </c>
     </row>
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>197</t>
+          <t>184</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>Kordell Norfleet , (Arizona State) DEC William Feldkamp , (Clarion), 13-8</t>
+          <t>Abe Assad , (Iowa) DEC Aj Burkhart , (Lehigh), 9-3</t>
         </is>
       </c>
     </row>
@@ -6095,7 +6095,7 @@
       </c>
       <c r="B479" t="inlineStr">
         <is>
-          <t>Jaron Smith , (Maryland) MD Evan Bockman , (Utah Valley), 16-4</t>
+          <t>Kordell Norfleet , (Arizona State) DEC William Feldkamp , (Clarion), 13-8</t>
         </is>
       </c>
     </row>
@@ -6107,7 +6107,7 @@
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>Tanner Sloan , (South Dakota State) DEC Andrew Davison , (Northwestern), 5-0</t>
+          <t>Jaron Smith , (Maryland) MD Evan Bockman , (Utah Valley), 16-4</t>
         </is>
       </c>
     </row>
@@ -6119,7 +6119,7 @@
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>Jacob Koser , (Navy) MD Benjamin Smith , (Cleveland State), 12-0</t>
+          <t>Tanner Sloan , (South Dakota State) DEC Andrew Davison , (Northwestern), 5-0</t>
         </is>
       </c>
     </row>
@@ -6131,7 +6131,7 @@
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>Jacob Cardenas , (Cornell) MD Cole Urbas , (Penn), 11-2</t>
+          <t>Jacob Koser , (Navy) MD Benjamin Smith , (Cleveland State), 12-0</t>
         </is>
       </c>
     </row>
@@ -6143,7 +6143,7 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>Owen Pentz , (North Dakota State) F Alan Clothier , (Northern Colorado), 2:13</t>
+          <t>Jacob Cardenas , (Cornell) MD Cole Urbas , (Penn), 11-2</t>
         </is>
       </c>
     </row>
@@ -6155,7 +6155,7 @@
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>Braxton Amos , (Wisconsin) DEC Michial Foy , (Minnesota), 2-0</t>
+          <t>Owen Pentz , (North Dakota State) F Alan Clothier , (Northern Colorado), 2:13</t>
         </is>
       </c>
     </row>
@@ -6167,19 +6167,19 @@
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>Isaac Trumble , (NC State) F J.t. Brown Elyria, OH (Army), 5:33</t>
+          <t>Braxton Amos , (Wisconsin) DEC Michial Foy , (Minnesota), 2-0</t>
         </is>
       </c>
     </row>
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>285</t>
+          <t>197</t>
         </is>
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>Trent Hillger , (Wisconsin) MD Tyrell Gordon , (Northern Iowa), 8-0</t>
+          <t>Isaac Trumble , (NC State) F J.t. Brown Elyria, OH (Army), 5:33</t>
         </is>
       </c>
     </row>
@@ -6191,7 +6191,7 @@
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>Isaac Reid , (Lock Haven) DEC Sam Schuyler , (Iowa State), 8-5</t>
+          <t>Trent Hillger , (Wisconsin) MD Tyrell Gordon , (Northern Iowa), 8-0</t>
         </is>
       </c>
     </row>
@@ -6203,7 +6203,7 @@
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>Tyrie Houghton , (NC State) DEC Michael Mcaleavey , (The Citadel), 9-4</t>
+          <t>Isaac Reid , (Lock Haven) DEC Sam Schuyler , (Iowa State), 8-5</t>
         </is>
       </c>
     </row>
@@ -6215,7 +6215,7 @@
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>Joe Doyle , (Binghamton) DEC Brandon Metz , (North Dakota State), 6-0</t>
+          <t>Tyrie Houghton , (NC State) DEC Michael Mcaleavey , (The Citadel), 9-4</t>
         </is>
       </c>
     </row>
@@ -6227,7 +6227,7 @@
       </c>
       <c r="B490" t="inlineStr">
         <is>
-          <t>Luke Surber , (Oklahoma State) DEC Josh Heindselman , (Oklahoma), 8-2</t>
+          <t>Joe Doyle , (Binghamton) DEC Brandon Metz , (North Dakota State), 6-0</t>
         </is>
       </c>
     </row>
@@ -6239,7 +6239,7 @@
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>Aj Nevills , (South Dakota State) DEC Michael Wolfgram , (West Virginia), 4-3</t>
+          <t>Luke Surber , (Oklahoma State) DEC Josh Heindselman , (Oklahoma), 8-2</t>
         </is>
       </c>
     </row>
@@ -6251,7 +6251,7 @@
       </c>
       <c r="B492" t="inlineStr">
         <is>
-          <t>Ben Goldin , (Penn) DEC Quinn Miller , (Virginia), 7-5</t>
+          <t>Aj Nevills , (South Dakota State) DEC Michael Wolfgram , (West Virginia), 4-3</t>
         </is>
       </c>
     </row>
@@ -6263,26 +6263,26 @@
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>Taye Ghadiali , (Campbell) DEC Zachary Knighton-ward , (Hofstra), 10-8</t>
+          <t>Ben Goldin , (Penn) DEC Quinn Miller , (Virginia), 7-5</t>
         </is>
       </c>
     </row>
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>ROUND OF 32</t>
+          <t>285</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Taye Ghadiali , (Campbell) DEC Zachary Knighton-ward , (Hofstra), 10-8</t>
         </is>
       </c>
     </row>
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>125</t>
-        </is>
-      </c>
-      <c r="B495" t="inlineStr">
-        <is>
-          <t>Nick Suriano , (Michigan) MD Logan Ashton , (Stanford), 16-3</t>
+          <t>ROUND OF 32</t>
         </is>
       </c>
     </row>
@@ -6294,7 +6294,7 @@
       </c>
       <c r="B496" t="inlineStr">
         <is>
-          <t>Anthony Noto , (Lock Haven) DEC Drew Hildebrandt , (Penn State), 4-2 SV</t>
+          <t>Nick Suriano , (Michigan) MD Logan Ashton , (Stanford), 16-3</t>
         </is>
       </c>
     </row>
@@ -6306,7 +6306,7 @@
       </c>
       <c r="B497" t="inlineStr">
         <is>
-          <t>Sam Latona , (Virginia Tech) DEC Devin Schroder , (Purdue), 4-1</t>
+          <t>Anthony Noto , (Lock Haven) DEC Drew Hildebrandt , (Penn State), 4-2 SV</t>
         </is>
       </c>
     </row>
@@ -6318,7 +6318,7 @@
       </c>
       <c r="B498" t="inlineStr">
         <is>
-          <t>Caleb Smith , (Appalachian State) DEC Patrick Mckee , (Minnesota), 8-5</t>
+          <t>Sam Latona , (Virginia Tech) DEC Devin Schroder , (Purdue), 4-1</t>
         </is>
       </c>
     </row>
@@ -6330,7 +6330,7 @@
       </c>
       <c r="B499" t="inlineStr">
         <is>
-          <t>Killian Cardinale , (West Virginia) MD Korbin Meink , (Campbell), 11-2</t>
+          <t>Caleb Smith , (Appalachian State) DEC Patrick Mckee , (Minnesota), 8-5</t>
         </is>
       </c>
     </row>
@@ -6342,7 +6342,7 @@
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>Taylor Lamont , (Utah Valley) DEC Malik Heinselman , (Ohio State), 7-2</t>
+          <t>Killian Cardinale , (West Virginia) MD Korbin Meink , (Campbell), 11-2</t>
         </is>
       </c>
     </row>
@@ -6354,7 +6354,7 @@
       </c>
       <c r="B501" t="inlineStr">
         <is>
-          <t>Fabian Gutierrez , (Chattanooga) DEC Drake Ayala , (Iowa), 12-9</t>
+          <t>Taylor Lamont , (Utah Valley) DEC Malik Heinselman , (Ohio State), 7-2</t>
         </is>
       </c>
     </row>
@@ -6366,7 +6366,7 @@
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>Brandon Courtney , (Arizona State) MD Joe Manchio , (Columbia), 14-5</t>
+          <t>Fabian Gutierrez , (Chattanooga) DEC Drake Ayala , (Iowa), 12-9</t>
         </is>
       </c>
     </row>
@@ -6378,7 +6378,7 @@
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>Pat Glory , (Princeton) MD Jace Koelzer , (Northern Colorado), 16-2</t>
+          <t>Brandon Courtney , (Arizona State) MD Joe Manchio , (Columbia), 14-5</t>
         </is>
       </c>
     </row>
@@ -6390,7 +6390,7 @@
       </c>
       <c r="B504" t="inlineStr">
         <is>
-          <t>Jakob Camacho , (NC State) DEC Joey Prata , (Oklahoma), 8-3</t>
+          <t>Pat Glory , (Princeton) MD Jace Koelzer , (Northern Colorado), 16-2</t>
         </is>
       </c>
     </row>
@@ -6402,7 +6402,7 @@
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>Brandon Kaylor , (Oregon State) MD Ryan Miller , (Penn), 16-4</t>
+          <t>Jakob Camacho , (NC State) DEC Joey Prata , (Oklahoma), 8-3</t>
         </is>
       </c>
     </row>
@@ -6414,7 +6414,7 @@
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>Eric Barnett , (Wisconsin) MD Justin Cardani , (Illinois), 9-0</t>
+          <t>Brandon Kaylor , (Oregon State) MD Ryan Miller , (Penn), 16-4</t>
         </is>
       </c>
     </row>
@@ -6426,7 +6426,7 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>Trevor Mastrogiovanni , (Oklahoma State) DEC Kysen Terukina , (Iowa State), 4-2</t>
+          <t>Eric Barnett , (Wisconsin) MD Justin Cardani , (Illinois), 9-0</t>
         </is>
       </c>
     </row>
@@ -6438,7 +6438,7 @@
       </c>
       <c r="B508" t="inlineStr">
         <is>
-          <t>Michael Deaugustino , (Northwestern) DEC Dylan Shawver , (Rutgers), 3-1</t>
+          <t>Trevor Mastrogiovanni , (Oklahoma State) DEC Kysen Terukina , (Iowa State), 4-2</t>
         </is>
       </c>
     </row>
@@ -6450,7 +6450,7 @@
       </c>
       <c r="B509" t="inlineStr">
         <is>
-          <t>Brody Teske , (Northern Iowa) DEC Noah Surtin , (Missouri), 5-3</t>
+          <t>Michael Deaugustino , (Northwestern) DEC Dylan Shawver , (Rutgers), 3-1</t>
         </is>
       </c>
     </row>
@@ -6462,19 +6462,19 @@
       </c>
       <c r="B510" t="inlineStr">
         <is>
-          <t>Vitali Arujau , (Cornell) MD Antonio Lorenzo , (California Poly), 16-4</t>
+          <t>Brody Teske , (Northern Iowa) DEC Noah Surtin , (Missouri), 5-3</t>
         </is>
       </c>
     </row>
     <row r="511">
       <c r="A511" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>125</t>
         </is>
       </c>
       <c r="B511" t="inlineStr">
         <is>
-          <t>Roman Bravo-young , (Penn State) MD Dominic Lajoie , (Cornell), 16-4</t>
+          <t>Vitali Arujau , (Cornell) MD Antonio Lorenzo , (California Poly), 16-4</t>
         </is>
       </c>
     </row>
@@ -6486,7 +6486,7 @@
       </c>
       <c r="B512" t="inlineStr">
         <is>
-          <t>Joshua Koderhandt , (Navy) DEC Haiden Drury , (Utah Valley), 5-4</t>
+          <t>Roman Bravo-young , (Penn State) MD Dominic Lajoie , (Cornell), 16-4</t>
         </is>
       </c>
     </row>
@@ -6498,7 +6498,7 @@
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>Michael Colaiocco , (Penn) DEF Ramazan Attasauov , (Iowa State)</t>
+          <t>Joshua Koderhandt , (Navy) DEC Haiden Drury , (Utah Valley), 5-4</t>
         </is>
       </c>
     </row>
@@ -6510,7 +6510,7 @@
       </c>
       <c r="B514" t="inlineStr">
         <is>
-          <t>Brian Courtney , (Virginia) DEC Rayvon Foley , (Michigan State), 4-2</t>
+          <t>Michael Colaiocco , (Penn) DEF Ramazan Attasauov , (Iowa State)</t>
         </is>
       </c>
     </row>
@@ -6522,7 +6522,7 @@
       </c>
       <c r="B515" t="inlineStr">
         <is>
-          <t>Austin Desanto , (Iowa) TF Sidney Flores , (Air Force), 19-3</t>
+          <t>Brian Courtney , (Virginia) DEC Rayvon Foley , (Michigan State), 4-2</t>
         </is>
       </c>
     </row>
@@ -6534,7 +6534,7 @@
       </c>
       <c r="B516" t="inlineStr">
         <is>
-          <t>Micky Phillippi , (Pittsburgh) DEC Codi Russell , (Appalachian State), 4-0</t>
+          <t>Austin Desanto , (Iowa) TF Sidney Flores , (Air Force), 19-3</t>
         </is>
       </c>
     </row>
@@ -6546,7 +6546,7 @@
       </c>
       <c r="B517" t="inlineStr">
         <is>
-          <t>Brock Hudkins , (Indiana) DEC Chance Rich , (Cal State Bakersfield), 8-3</t>
+          <t>Micky Phillippi , (Pittsburgh) DEC Codi Russell , (Appalachian State), 4-0</t>
         </is>
       </c>
     </row>
@@ -6558,7 +6558,7 @@
       </c>
       <c r="B518" t="inlineStr">
         <is>
-          <t>Korbin Myers , (Virginia Tech) MD Jake Gliva , (Minnesota), 12-0</t>
+          <t>Brock Hudkins , (Indiana) DEC Chance Rich , (Cal State Bakersfield), 8-3</t>
         </is>
       </c>
     </row>
@@ -6570,7 +6570,7 @@
       </c>
       <c r="B519" t="inlineStr">
         <is>
-          <t>Michael Mcgee , (Arizona State) TF Richie Koehler , (Rider), 18-3</t>
+          <t>Korbin Myers , (Virginia Tech) MD Jake Gliva , (Minnesota), 12-0</t>
         </is>
       </c>
     </row>
@@ -6582,7 +6582,7 @@
       </c>
       <c r="B520" t="inlineStr">
         <is>
-          <t>Kyle Biscoglia , (Northern Iowa) F Brayden Palmer , (Chattanooga), 2:35</t>
+          <t>Michael Mcgee , (Arizona State) TF Richie Koehler , (Rider), 18-3</t>
         </is>
       </c>
     </row>
@@ -6594,7 +6594,7 @@
       </c>
       <c r="B521" t="inlineStr">
         <is>
-          <t>Devan Turner , (Oregon State) DEC Joe Olivieri , (Rutgers), 10-4</t>
+          <t>Kyle Biscoglia , (Northern Iowa) F Brayden Palmer , (Chattanooga), 2:35</t>
         </is>
       </c>
     </row>
@@ -6606,7 +6606,7 @@
       </c>
       <c r="B522" t="inlineStr">
         <is>
-          <t>Dylan Ragusin , (Michigan) DEC Malyke Hines , (Lehigh), 8-5</t>
+          <t>Devan Turner , (Oregon State) DEC Joe Olivieri , (Rutgers), 10-4</t>
         </is>
       </c>
     </row>
@@ -6618,7 +6618,7 @@
       </c>
       <c r="B523" t="inlineStr">
         <is>
-          <t>Matt Ramos , (Purdue) F Lucas Byrd , (Illinois), 2:27</t>
+          <t>Dylan Ragusin , (Michigan) DEC Malyke Hines , (Lehigh), 8-5</t>
         </is>
       </c>
     </row>
@@ -6630,7 +6630,7 @@
       </c>
       <c r="B524" t="inlineStr">
         <is>
-          <t>Chris Cannon , (Northwestern) DEC Anthony Madrigal , (Oklahoma), 3-1</t>
+          <t>Matt Ramos , (Purdue) F Lucas Byrd , (Illinois), 2:27</t>
         </is>
       </c>
     </row>
@@ -6642,7 +6642,7 @@
       </c>
       <c r="B525" t="inlineStr">
         <is>
-          <t>Kai Orine , (NC State) DEC Joseph Heilmann , (North Carolina), 4-3</t>
+          <t>Chris Cannon , (Northwestern) DEC Anthony Madrigal , (Oklahoma), 3-1</t>
         </is>
       </c>
     </row>
@@ -6654,19 +6654,19 @@
       </c>
       <c r="B526" t="inlineStr">
         <is>
-          <t>Daton Fix , (Oklahoma State) MD Kyle Burwick , (Wisconsin), 20-8</t>
+          <t>Kai Orine , (NC State) DEC Joseph Heilmann , (North Carolina), 4-3</t>
         </is>
       </c>
     </row>
     <row r="527">
       <c r="A527" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>133</t>
         </is>
       </c>
       <c r="B527" t="inlineStr">
         <is>
-          <t>Nick Lee , (Penn State) MD Josh Mason , (Bloomsburg), 15-3</t>
+          <t>Daton Fix , (Oklahoma State) MD Kyle Burwick , (Wisconsin), 20-8</t>
         </is>
       </c>
     </row>
@@ -6678,7 +6678,7 @@
       </c>
       <c r="B528" t="inlineStr">
         <is>
-          <t>Quinn Kinner , (Rider) DEC Dylan D`emilio , (Ohio State), 3-0</t>
+          <t>Nick Lee , (Penn State) MD Josh Mason , (Bloomsburg), 15-3</t>
         </is>
       </c>
     </row>
@@ -6690,7 +6690,7 @@
       </c>
       <c r="B529" t="inlineStr">
         <is>
-          <t>Allan Hart , (Missouri) DEC Stevan Micic , (Michigan), 7-3</t>
+          <t>Quinn Kinner , (Rider) DEC Dylan D`emilio , (Ohio State), 3-0</t>
         </is>
       </c>
     </row>
@@ -6702,7 +6702,7 @@
       </c>
       <c r="B530" t="inlineStr">
         <is>
-          <t>Grant Willits , (Oregon State) DEC Carter Young , (Oklahoma State), 5-3</t>
+          <t>Allan Hart , (Missouri) DEC Stevan Micic , (Michigan), 7-3</t>
         </is>
       </c>
     </row>
@@ -6714,7 +6714,7 @@
       </c>
       <c r="B531" t="inlineStr">
         <is>
-          <t>Andrew Alirez , (Northern Colorado) DEC Collin Gerardi , (Virginia Tech), 5-1</t>
+          <t>Grant Willits , (Oregon State) DEC Carter Young , (Oklahoma State), 5-3</t>
         </is>
       </c>
     </row>
@@ -6726,7 +6726,7 @@
       </c>
       <c r="B532" t="inlineStr">
         <is>
-          <t>Cj Composto , (Penn) DEC Dylan Droegemueller , (North Dakota State), 7-4</t>
+          <t>Andrew Alirez , (Northern Colorado) DEC Collin Gerardi , (Virginia Tech), 5-1</t>
         </is>
       </c>
     </row>
@@ -6738,7 +6738,7 @@
       </c>
       <c r="B533" t="inlineStr">
         <is>
-          <t>Parker Filius , (Purdue) MD Ian Parker , (Iowa State), 13-5</t>
+          <t>Cj Composto , (Penn) DEC Dylan Droegemueller , (North Dakota State), 7-4</t>
         </is>
       </c>
     </row>
@@ -6750,7 +6750,7 @@
       </c>
       <c r="B534" t="inlineStr">
         <is>
-          <t>Real Woods , (Stanford) MD Connor Mcgonagle , (Lehigh), 8-0</t>
+          <t>Parker Filius , (Purdue) MD Ian Parker , (Iowa State), 13-5</t>
         </is>
       </c>
     </row>
@@ -6762,7 +6762,7 @@
       </c>
       <c r="B535" t="inlineStr">
         <is>
-          <t>Sebastian Rivera , (Rutgers) MD Jacob Butler , (Oklahoma), 12-3</t>
+          <t>Real Woods , (Stanford) MD Connor Mcgonagle , (Lehigh), 8-0</t>
         </is>
       </c>
     </row>
@@ -6774,7 +6774,7 @@
       </c>
       <c r="B536" t="inlineStr">
         <is>
-          <t>Chad Red , (Nebraska) DEC Dresden Simon , (Central Michigan), 6-5</t>
+          <t>Sebastian Rivera , (Rutgers) MD Jacob Butler , (Oklahoma), 12-3</t>
         </is>
       </c>
     </row>
@@ -6786,7 +6786,7 @@
       </c>
       <c r="B537" t="inlineStr">
         <is>
-          <t>Matt Kazimir , (Columbia) DEC Shannon Hanna , (Campbell), 5-2</t>
+          <t>Chad Red , (Nebraska) DEC Dresden Simon , (Central Michigan), 6-5</t>
         </is>
       </c>
     </row>
@@ -6798,7 +6798,7 @@
       </c>
       <c r="B538" t="inlineStr">
         <is>
-          <t>Cole Matthews , (Pittsburgh) DEC Joseph Zargo , (Wisconsin), 12-8</t>
+          <t>Matt Kazimir , (Columbia) DEC Shannon Hanna , (Campbell), 5-2</t>
         </is>
       </c>
     </row>
@@ -6810,7 +6810,7 @@
       </c>
       <c r="B539" t="inlineStr">
         <is>
-          <t>Frankie Tal sharar , (Northwestern) DEC Clay Carlson , (South Dakota State), 4-3</t>
+          <t>Cole Matthews , (Pittsburgh) DEC Joseph Zargo , (Wisconsin), 12-8</t>
         </is>
       </c>
     </row>
@@ -6822,7 +6822,7 @@
       </c>
       <c r="B540" t="inlineStr">
         <is>
-          <t>Jake Bergeland , (Minnesota) MD Gabe Willochell , (Edinboro), 9-1</t>
+          <t>Frankie Tal sharar , (Northwestern) DEC Clay Carlson , (South Dakota State), 4-3</t>
         </is>
       </c>
     </row>
@@ -6834,7 +6834,7 @@
       </c>
       <c r="B541" t="inlineStr">
         <is>
-          <t>Kizhan Clarke , (North Carolina) DEC Ryan Jack , (NC State), 4-3</t>
+          <t>Jake Bergeland , (Minnesota) MD Gabe Willochell , (Edinboro), 9-1</t>
         </is>
       </c>
     </row>
@@ -6846,19 +6846,19 @@
       </c>
       <c r="B542" t="inlineStr">
         <is>
-          <t>Jaydin Eierman , (Iowa) DEC Wilfredo Gil , (Franklin &amp; Marshall), 11-4</t>
+          <t>Kizhan Clarke , (North Carolina) DEC Ryan Jack , (NC State), 4-3</t>
         </is>
       </c>
     </row>
     <row r="543">
       <c r="A543" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>141</t>
         </is>
       </c>
       <c r="B543" t="inlineStr">
         <is>
-          <t>Yianni Diakomihalis , (Cornell) DEC Zachary Sherman , (North Carolina), 9-2</t>
+          <t>Jaydin Eierman , (Iowa) DEC Wilfredo Gil , (Franklin &amp; Marshall), 11-4</t>
         </is>
       </c>
     </row>
@@ -6870,7 +6870,7 @@
       </c>
       <c r="B544" t="inlineStr">
         <is>
-          <t>Willie Mcdougald , (Oklahoma) DEC Jarrett Degen , (Iowa State), 10-7</t>
+          <t>Yianni Diakomihalis , (Cornell) DEC Zachary Sherman , (North Carolina), 9-2</t>
         </is>
       </c>
     </row>
@@ -6882,7 +6882,7 @@
       </c>
       <c r="B545" t="inlineStr">
         <is>
-          <t>Kaden Gfeller , (Oklahoma State) DEC Pj Ogunsanya , (Army), 7-1</t>
+          <t>Willie Mcdougald , (Oklahoma) DEC Jarrett Degen , (Iowa State), 10-7</t>
         </is>
       </c>
     </row>
@@ -6894,7 +6894,7 @@
       </c>
       <c r="B546" t="inlineStr">
         <is>
-          <t>Max Murin , (Iowa) F Corbyn Munson , (Central Michigan), 4:49</t>
+          <t>Kaden Gfeller , (Oklahoma State) DEC Pj Ogunsanya , (Army), 7-1</t>
         </is>
       </c>
     </row>
@@ -6906,7 +6906,7 @@
       </c>
       <c r="B547" t="inlineStr">
         <is>
-          <t>Kyle Parco , (Arizona State) MD Kody Komara , (Kent State), 14-3</t>
+          <t>Max Murin , (Iowa) F Corbyn Munson , (Central Michigan), 4:49</t>
         </is>
       </c>
     </row>
@@ -6918,7 +6918,7 @@
       </c>
       <c r="B548" t="inlineStr">
         <is>
-          <t>Marcus Robinson , (Cleveland State) DEC Mike Van brill , (Rutgers), 7-5</t>
+          <t>Kyle Parco , (Arizona State) MD Kody Komara , (Kent State), 14-3</t>
         </is>
       </c>
     </row>
@@ -6930,7 +6930,7 @@
       </c>
       <c r="B549" t="inlineStr">
         <is>
-          <t>Beau Bartlett , (Penn State) DEC Colin Realbuto , (Northern Iowa), 5-4</t>
+          <t>Marcus Robinson , (Cleveland State) DEC Mike Van brill , (Rutgers), 7-5</t>
         </is>
       </c>
     </row>
@@ -6942,7 +6942,7 @@
       </c>
       <c r="B550" t="inlineStr">
         <is>
-          <t>Sammy Sasso , (Ohio State) DEC John Arceri , (Buffalo), 5-0</t>
+          <t>Beau Bartlett , (Penn State) DEC Colin Realbuto , (Northern Iowa), 5-4</t>
         </is>
       </c>
     </row>
@@ -6954,7 +6954,7 @@
       </c>
       <c r="B551" t="inlineStr">
         <is>
-          <t>Austin Gomez , (Wisconsin) MD Marshall Keller , (Princeton), 12-0</t>
+          <t>Sammy Sasso , (Ohio State) DEC John Arceri , (Buffalo), 5-0</t>
         </is>
       </c>
     </row>
@@ -6966,7 +6966,7 @@
       </c>
       <c r="B552" t="inlineStr">
         <is>
-          <t>Josh Finesilver , (Duke) DEC Yahya Thomas , (Northwestern), 13-10</t>
+          <t>Austin Gomez , (Wisconsin) MD Marshall Keller , (Princeton), 12-0</t>
         </is>
       </c>
     </row>
@@ -6978,7 +6978,7 @@
       </c>
       <c r="B553" t="inlineStr">
         <is>
-          <t>Bryce Andonian , (Virginia Tech) DEC Max Brignola , (Lehigh), 9-7</t>
+          <t>Josh Finesilver , (Duke) DEC Yahya Thomas , (Northwestern), 13-10</t>
         </is>
       </c>
     </row>
@@ -6990,7 +6990,7 @@
       </c>
       <c r="B554" t="inlineStr">
         <is>
-          <t>Jonathan Millner , (Appalachian State) DEC Cory Crooks , (Oregon State), 3-0</t>
+          <t>Bryce Andonian , (Virginia Tech) DEC Max Brignola , (Lehigh), 9-7</t>
         </is>
       </c>
     </row>
@@ -7002,7 +7002,7 @@
       </c>
       <c r="B555" t="inlineStr">
         <is>
-          <t>Joshua Heil , (Campbell) MD Joshua Edmond , (Missouri), 8-0</t>
+          <t>Jonathan Millner , (Appalachian State) DEC Cory Crooks , (Oregon State), 3-0</t>
         </is>
       </c>
     </row>
@@ -7014,7 +7014,7 @@
       </c>
       <c r="B556" t="inlineStr">
         <is>
-          <t>Ridge Lovett , (Nebraska) DEC Jaden Abas , (Stanford), 4-2</t>
+          <t>Joshua Heil , (Campbell) MD Joshua Edmond , (Missouri), 8-0</t>
         </is>
       </c>
     </row>
@@ -7026,7 +7026,7 @@
       </c>
       <c r="B557" t="inlineStr">
         <is>
-          <t>Anthony Artalona , (Penn) DEC Legend Lamer , (California Poly), 3-2</t>
+          <t>Ridge Lovett , (Nebraska) DEC Jaden Abas , (Stanford), 4-2</t>
         </is>
       </c>
     </row>
@@ -7038,19 +7038,19 @@
       </c>
       <c r="B558" t="inlineStr">
         <is>
-          <t>Tariq Wilson , (NC State) DEC Michael Blockhus , (Minnesota), 5-3</t>
+          <t>Anthony Artalona , (Penn) DEC Legend Lamer , (California Poly), 3-2</t>
         </is>
       </c>
     </row>
     <row r="559">
       <c r="A559" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>149</t>
         </is>
       </c>
       <c r="B559" t="inlineStr">
         <is>
-          <t>David Carr , (Iowa State) TF Derek Holschlag , (Northern Iowa), 21-6</t>
+          <t>Tariq Wilson , (NC State) DEC Michael Blockhus , (Minnesota), 5-3</t>
         </is>
       </c>
     </row>
@@ -7062,7 +7062,7 @@
       </c>
       <c r="B560" t="inlineStr">
         <is>
-          <t>Hunter Willits , (Oregon State) DEC Brady Berge , (Penn State), 2-1</t>
+          <t>David Carr , (Iowa State) TF Derek Holschlag , (Northern Iowa), 21-6</t>
         </is>
       </c>
     </row>
@@ -7074,7 +7074,7 @@
       </c>
       <c r="B561" t="inlineStr">
         <is>
-          <t>Kaleb Young , (Iowa) DEC Doug Zapf , (Penn), 3-2</t>
+          <t>Hunter Willits , (Oregon State) DEC Brady Berge , (Penn State), 2-1</t>
         </is>
       </c>
     </row>
@@ -7086,7 +7086,7 @@
       </c>
       <c r="B562" t="inlineStr">
         <is>
-          <t>Will Lewan , (Michigan) DEC Jarrett Jacques , (Missouri), 4-2 SV</t>
+          <t>Kaleb Young , (Iowa) DEC Doug Zapf , (Penn), 3-2</t>
         </is>
       </c>
     </row>
@@ -7098,7 +7098,7 @@
       </c>
       <c r="B563" t="inlineStr">
         <is>
-          <t>Quincy Monday , (Princeton) DEC Connor Brady , (Virginia Tech), 3-2</t>
+          <t>Will Lewan , (Michigan) DEC Jarrett Jacques , (Missouri), 4-2 SV</t>
         </is>
       </c>
     </row>
@@ -7110,7 +7110,7 @@
       </c>
       <c r="B564" t="inlineStr">
         <is>
-          <t>Jacob Wright , (Wyoming) DEC Chase Saldate , (Michigan State), 6-1</t>
+          <t>Quincy Monday , (Princeton) DEC Connor Brady , (Virginia Tech), 3-2</t>
         </is>
       </c>
     </row>
@@ -7122,7 +7122,7 @@
       </c>
       <c r="B565" t="inlineStr">
         <is>
-          <t>Justin Thomas , (Oklahoma) DEC Elijah Cleary , (Pittsburgh), 6-5</t>
+          <t>Jacob Wright , (Wyoming) DEC Chase Saldate , (Michigan State), 6-1</t>
         </is>
       </c>
     </row>
@@ -7134,7 +7134,7 @@
       </c>
       <c r="B566" t="inlineStr">
         <is>
-          <t>Ed Scott , (NC State) F Michael Petite , (Buffalo), 4:45</t>
+          <t>Justin Thomas , (Oklahoma) DEC Elijah Cleary , (Pittsburgh), 6-5</t>
         </is>
       </c>
     </row>
@@ -7146,7 +7146,7 @@
       </c>
       <c r="B567" t="inlineStr">
         <is>
-          <t>Jacori Teemer , (Arizona State) DEC Hunter Richard , (Cornell), 3-2</t>
+          <t>Ed Scott , (NC State) F Michael Petite , (Buffalo), 4:45</t>
         </is>
       </c>
     </row>
@@ -7158,7 +7158,7 @@
       </c>
       <c r="B568" t="inlineStr">
         <is>
-          <t>Jake Keating , (Virginia) DEC Kendall Coleman , (Purdue), 6-2</t>
+          <t>Jacori Teemer , (Arizona State) DEC Hunter Richard , (Cornell), 3-2</t>
         </is>
       </c>
     </row>
@@ -7170,7 +7170,7 @@
       </c>
       <c r="B569" t="inlineStr">
         <is>
-          <t>Dazjon Casto , (The Citadel) DEC Austin O`connor , (North Carolina), 8-2 SV</t>
+          <t>Jake Keating , (Virginia) DEC Kendall Coleman , (Purdue), 6-2</t>
         </is>
       </c>
     </row>
@@ -7182,7 +7182,7 @@
       </c>
       <c r="B570" t="inlineStr">
         <is>
-          <t>Jared Franek , (North Dakota State) MD Garrett Model , (Wisconsin), 10-0</t>
+          <t>Dazjon Casto , (The Citadel) DEC Austin O`connor , (North Carolina), 8-2 SV</t>
         </is>
       </c>
     </row>
@@ -7194,7 +7194,7 @@
       </c>
       <c r="B571" t="inlineStr">
         <is>
-          <t>Josh Humphreys , (Lehigh) DEC Ben Barton , (Lock Haven), 4-0</t>
+          <t>Jared Franek , (North Dakota State) MD Garrett Model , (Wisconsin), 10-0</t>
         </is>
       </c>
     </row>
@@ -7206,7 +7206,7 @@
       </c>
       <c r="B572" t="inlineStr">
         <is>
-          <t>Peyton Robb , (Nebraska) F Markus Hartman , (Army), 1:51</t>
+          <t>Josh Humphreys , (Lehigh) DEC Ben Barton , (Lock Haven), 4-0</t>
         </is>
       </c>
     </row>
@@ -7218,7 +7218,7 @@
       </c>
       <c r="B573" t="inlineStr">
         <is>
-          <t>Johnny Lovett , (Central Michigan) DEC Andrew Cerniglia , (Navy), 6-5</t>
+          <t>Peyton Robb , (Nebraska) F Markus Hartman , (Army), 1:51</t>
         </is>
       </c>
     </row>
@@ -7230,19 +7230,19 @@
       </c>
       <c r="B574" t="inlineStr">
         <is>
-          <t>Ryan Deakin , (Northwestern) DEC Wyatt Sheets , (Oklahoma State), 6-2</t>
+          <t>Johnny Lovett , (Central Michigan) DEC Andrew Cerniglia , (Navy), 6-5</t>
         </is>
       </c>
     </row>
     <row r="575">
       <c r="A575" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>157</t>
         </is>
       </c>
       <c r="B575" t="inlineStr">
         <is>
-          <t>Evan Wick , (California Poly) MD Matthew Olguin , (Oregon State), 11-3</t>
+          <t>Ryan Deakin , (Northwestern) DEC Wyatt Sheets , (Oklahoma State), 6-2</t>
         </is>
       </c>
     </row>
@@ -7254,7 +7254,7 @@
       </c>
       <c r="B576" t="inlineStr">
         <is>
-          <t>Luke Weber , (North Dakota State) DEC Brian Meyer , (Lehigh), 3-0</t>
+          <t>Evan Wick , (California Poly) MD Matthew Olguin , (Oregon State), 11-3</t>
         </is>
       </c>
     </row>
@@ -7266,7 +7266,7 @@
       </c>
       <c r="B577" t="inlineStr">
         <is>
-          <t>Peyton Hall , (West Virginia) DEC Riley Smucker , (Cleveland State), 10-5</t>
+          <t>Luke Weber , (North Dakota State) DEC Brian Meyer , (Lehigh), 3-0</t>
         </is>
       </c>
     </row>
@@ -7278,7 +7278,7 @@
       </c>
       <c r="B578" t="inlineStr">
         <is>
-          <t>Philip Conigliaro , (Harvard) DEC Brevin Cassella , (Binghamton), 6-4</t>
+          <t>Peyton Hall , (West Virginia) DEC Riley Smucker , (Cleveland State), 10-5</t>
         </is>
       </c>
     </row>
@@ -7290,7 +7290,7 @@
       </c>
       <c r="B579" t="inlineStr">
         <is>
-          <t>Shane Griffith , (Stanford) TF Cael Carlson , (Minnesota), 18-2</t>
+          <t>Philip Conigliaro , (Harvard) DEC Brevin Cassella , (Binghamton), 6-4</t>
         </is>
       </c>
     </row>
@@ -7302,7 +7302,7 @@
       </c>
       <c r="B580" t="inlineStr">
         <is>
-          <t>Zach Hartman , (Bucknell) DEC Thomas Bullard , (NC State), 5-1</t>
+          <t>Shane Griffith , (Stanford) TF Cael Carlson , (Minnesota), 18-2</t>
         </is>
       </c>
     </row>
@@ -7314,7 +7314,7 @@
       </c>
       <c r="B581" t="inlineStr">
         <is>
-          <t>Julian Ramirez , (Cornell) DEC William Formato , (Appalachian State), 8-3</t>
+          <t>Zach Hartman , (Bucknell) DEC Thomas Bullard , (NC State), 5-1</t>
         </is>
       </c>
     </row>
@@ -7326,7 +7326,7 @@
       </c>
       <c r="B582" t="inlineStr">
         <is>
-          <t>Dean Hamiti , (Wisconsin) F Andrew Nicholson , (Chattanooga), 4:19</t>
+          <t>Julian Ramirez , (Cornell) DEC William Formato , (Appalachian State), 8-3</t>
         </is>
       </c>
     </row>
@@ -7338,7 +7338,7 @@
       </c>
       <c r="B583" t="inlineStr">
         <is>
-          <t>Alex Marinelli , (Iowa) DEC Evan Barczak , (Drexel), 7-2</t>
+          <t>Dean Hamiti , (Wisconsin) F Andrew Nicholson , (Chattanooga), 4:19</t>
         </is>
       </c>
     </row>
@@ -7350,7 +7350,7 @@
       </c>
       <c r="B584" t="inlineStr">
         <is>
-          <t>Justin Mccoy , (Virginia) DEC Joshua Ogunsanya , (Columbia), 6-1</t>
+          <t>Alex Marinelli , (Iowa) DEC Evan Barczak , (Drexel), 7-2</t>
         </is>
       </c>
     </row>
@@ -7362,7 +7362,7 @@
       </c>
       <c r="B585" t="inlineStr">
         <is>
-          <t>Izzak Olejnik , (Northern Illinois) DEC Rodrick Mosley , (Gardner-Webb), 2-1 TB1</t>
+          <t>Justin Mccoy , (Virginia) DEC Joshua Ogunsanya , (Columbia), 6-1</t>
         </is>
       </c>
     </row>
@@ -7374,7 +7374,7 @@
       </c>
       <c r="B586" t="inlineStr">
         <is>
-          <t>Cameron Amine , (Michigan) DEC Clayton Wilson , (Nebraska), 3-1</t>
+          <t>Izzak Olejnik , (Northern Illinois) DEC Rodrick Mosley , (Gardner-Webb), 2-1 TB1</t>
         </is>
       </c>
     </row>
@@ -7386,7 +7386,7 @@
       </c>
       <c r="B587" t="inlineStr">
         <is>
-          <t>Carson Kharchla , (Ohio State) DEC Lucas Revano , (Penn), 8-2</t>
+          <t>Cameron Amine , (Michigan) DEC Clayton Wilson , (Nebraska), 3-1</t>
         </is>
       </c>
     </row>
@@ -7398,7 +7398,7 @@
       </c>
       <c r="B588" t="inlineStr">
         <is>
-          <t>Jake Wentzel , (Pittsburgh) F Ashton Eyler , (Lock Haven), 2:56</t>
+          <t>Carson Kharchla , (Ohio State) DEC Lucas Revano , (Penn), 8-2</t>
         </is>
       </c>
     </row>
@@ -7410,7 +7410,7 @@
       </c>
       <c r="B589" t="inlineStr">
         <is>
-          <t>Anthony Valencia , (Arizona State) DEC Austin Yant , (Northern Iowa), 6-3</t>
+          <t>Jake Wentzel , (Pittsburgh) F Ashton Eyler , (Lock Haven), 2:56</t>
         </is>
       </c>
     </row>
@@ -7422,19 +7422,19 @@
       </c>
       <c r="B590" t="inlineStr">
         <is>
-          <t>Keegan O`toole , (Missouri) F Caleb Fish , (Michigan State), 0:52</t>
+          <t>Anthony Valencia , (Arizona State) DEC Austin Yant , (Northern Iowa), 6-3</t>
         </is>
       </c>
     </row>
     <row r="591">
       <c r="A591" t="inlineStr">
         <is>
-          <t>174</t>
+          <t>165</t>
         </is>
       </c>
       <c r="B591" t="inlineStr">
         <is>
-          <t>Carter Starocci , (Penn State) F Connor Oneill , (Rutgers), 6:39</t>
+          <t>Keegan O`toole , (Missouri) F Caleb Fish , (Michigan State), 0:52</t>
         </is>
       </c>
     </row>
@@ -7446,7 +7446,7 @@
       </c>
       <c r="B592" t="inlineStr">
         <is>
-          <t>Adam Kemp , (California Poly) DEC Nick Incontrera , (Penn), 6-5</t>
+          <t>Carter Starocci , (Penn State) F Connor Oneill , (Rutgers), 6:39</t>
         </is>
       </c>
     </row>
@@ -7458,7 +7458,7 @@
       </c>
       <c r="B593" t="inlineStr">
         <is>
-          <t>Mikey Labriola , (Nebraska) DEC Joel Devine , (Iowa State), 5-2</t>
+          <t>Adam Kemp , (California Poly) DEC Nick Incontrera , (Penn), 6-5</t>
         </is>
       </c>
     </row>
@@ -7470,7 +7470,7 @@
       </c>
       <c r="B594" t="inlineStr">
         <is>
-          <t>Gerrit Nijenhuis , (Purdue) DEC Michael O'malley Hasbrouck Heights, NJ (Drexel), 6-4 SV</t>
+          <t>Mikey Labriola , (Nebraska) DEC Joel Devine , (Iowa State), 5-2</t>
         </is>
       </c>
     </row>
@@ -7482,7 +7482,7 @@
       </c>
       <c r="B595" t="inlineStr">
         <is>
-          <t>Michael Kemerer , (Iowa) DEC Benjamin Pasiuk , (Army), 4-0</t>
+          <t>Gerrit Nijenhuis , (Purdue) DEC Michael O'malley Hasbrouck Heights, NJ (Drexel), 6-4 SV</t>
         </is>
       </c>
     </row>
@@ -7494,7 +7494,7 @@
       </c>
       <c r="B596" t="inlineStr">
         <is>
-          <t>Cade Devos , (South Dakota State) DEC Bailee O`reilly , (Minnesota), 9-2</t>
+          <t>Michael Kemerer , (Iowa) DEC Benjamin Pasiuk , (Army), 4-0</t>
         </is>
       </c>
     </row>
@@ -7506,7 +7506,7 @@
       </c>
       <c r="B597" t="inlineStr">
         <is>
-          <t>Matthew Finesilver , (Duke) DEC Hayden Hastings , (Wyoming), 5-3</t>
+          <t>Cade Devos , (South Dakota State) DEC Bailee O`reilly , (Minnesota), 9-2</t>
         </is>
       </c>
     </row>
@@ -7518,7 +7518,7 @@
       </c>
       <c r="B598" t="inlineStr">
         <is>
-          <t>Hayden Hidlay , (NC State) F Jay Nivison Buffalo, NY (Buffalo), 2:43</t>
+          <t>Matthew Finesilver , (Duke) DEC Hayden Hastings , (Wyoming), 5-3</t>
         </is>
       </c>
     </row>
@@ -7530,7 +7530,7 @@
       </c>
       <c r="B599" t="inlineStr">
         <is>
-          <t>Logan Massa , (Michigan) MD Jacob Nolan , (Binghamton), 12-4</t>
+          <t>Hayden Hidlay , (NC State) F Jay Nivison Buffalo, NY (Buffalo), 2:43</t>
         </is>
       </c>
     </row>
@@ -7542,7 +7542,7 @@
       </c>
       <c r="B600" t="inlineStr">
         <is>
-          <t>Thomas Flitz , (Appalachian State) DEC Christopher Foca , (Cornell), 9-6</t>
+          <t>Logan Massa , (Michigan) MD Jacob Nolan , (Binghamton), 12-4</t>
         </is>
       </c>
     </row>
@@ -7554,7 +7554,7 @@
       </c>
       <c r="B601" t="inlineStr">
         <is>
-          <t>Mason Kauffman , (Northern Illinois) DEC Peyton Mocco , (Missouri), 3-1</t>
+          <t>Thomas Flitz , (Appalachian State) DEC Christopher Foca , (Cornell), 9-6</t>
         </is>
       </c>
     </row>
@@ -7566,7 +7566,7 @@
       </c>
       <c r="B602" t="inlineStr">
         <is>
-          <t>Dustin Plott , (Oklahoma State) DEC Sal Perrine , (Ohio), 8-2</t>
+          <t>Mason Kauffman , (Northern Illinois) DEC Peyton Mocco , (Missouri), 3-1</t>
         </is>
       </c>
     </row>
@@ -7578,7 +7578,7 @@
       </c>
       <c r="B603" t="inlineStr">
         <is>
-          <t>Tyler Eischens , (Stanford) DEC Ethan Smith , (Ohio State), 13-12</t>
+          <t>Dustin Plott , (Oklahoma State) DEC Sal Perrine , (Ohio), 8-2</t>
         </is>
       </c>
     </row>
@@ -7590,7 +7590,7 @@
       </c>
       <c r="B604" t="inlineStr">
         <is>
-          <t>Clay Lautt , (North Carolina) DEC Troy Fisher , (Northwestern), 8-1</t>
+          <t>Tyler Eischens , (Stanford) DEC Ethan Smith , (Ohio State), 13-12</t>
         </is>
       </c>
     </row>
@@ -7602,7 +7602,7 @@
       </c>
       <c r="B605" t="inlineStr">
         <is>
-          <t>Lance Runyon , (Northern Iowa) F Anthony Mantanona , (Oklahoma), 4:14</t>
+          <t>Clay Lautt , (North Carolina) DEC Troy Fisher , (Northwestern), 8-1</t>
         </is>
       </c>
     </row>
@@ -7614,19 +7614,19 @@
       </c>
       <c r="B606" t="inlineStr">
         <is>
-          <t>Mekhi Lewis , (Virginia Tech) MD Dennis Robin , (West Virginia), 15-7</t>
+          <t>Lance Runyon , (Northern Iowa) F Anthony Mantanona , (Oklahoma), 4:14</t>
         </is>
       </c>
     </row>
     <row r="607">
       <c r="A607" t="inlineStr">
         <is>
-          <t>184</t>
+          <t>174</t>
         </is>
       </c>
       <c r="B607" t="inlineStr">
         <is>
-          <t>Myles Amine , (Michigan) TF Colin Mccracken , (Kent State), 18-3</t>
+          <t>Mekhi Lewis , (Virginia Tech) MD Dennis Robin , (West Virginia), 15-7</t>
         </is>
       </c>
     </row>
@@ -7638,7 +7638,7 @@
       </c>
       <c r="B608" t="inlineStr">
         <is>
-          <t>Dakota Geer , (Oklahoma State) F Jeremiah Kent , (Missouri), 6:26</t>
+          <t>Myles Amine , (Michigan) TF Colin Mccracken , (Kent State), 18-3</t>
         </is>
       </c>
     </row>
@@ -7650,7 +7650,7 @@
       </c>
       <c r="B609" t="inlineStr">
         <is>
-          <t>Zach Braunagel , (Illinois) DEC Caleb Hopkins , (Campbell), 11-4</t>
+          <t>Dakota Geer , (Oklahoma State) F Jeremiah Kent , (Missouri), 6:26</t>
         </is>
       </c>
     </row>
@@ -7662,7 +7662,7 @@
       </c>
       <c r="B610" t="inlineStr">
         <is>
-          <t>Marcus Coleman , (Iowa State) MD Michael Battista , (Virginia), 10-2</t>
+          <t>Zach Braunagel , (Illinois) DEC Caleb Hopkins , (Campbell), 11-4</t>
         </is>
       </c>
     </row>
@@ -7674,7 +7674,7 @@
       </c>
       <c r="B611" t="inlineStr">
         <is>
-          <t>Bernie Truax , (California Poly) DEC Gregg Harvey , (Pittsburgh), 1-0</t>
+          <t>Marcus Coleman , (Iowa State) MD Michael Battista , (Virginia), 10-2</t>
         </is>
       </c>
     </row>
@@ -7686,7 +7686,7 @@
       </c>
       <c r="B612" t="inlineStr">
         <is>
-          <t>Tate Samuelson , (Wyoming) DEC Brit Wilson , (Northern Illinois), 5-3 SV</t>
+          <t>Bernie Truax , (California Poly) DEC Gregg Harvey , (Pittsburgh), 1-0</t>
         </is>
       </c>
     </row>
@@ -7698,7 +7698,7 @@
       </c>
       <c r="B613" t="inlineStr">
         <is>
-          <t>Kyle Cochran , (Maryland) DEC John Poznanski , (Rutgers), 7-3</t>
+          <t>Tate Samuelson , (Wyoming) DEC Brit Wilson , (Northern Illinois), 5-3 SV</t>
         </is>
       </c>
     </row>
@@ -7710,7 +7710,7 @@
       </c>
       <c r="B614" t="inlineStr">
         <is>
-          <t>Parker Keckeisen , (Northern Iowa) MD Christopher Weiler , (Wisconsin), 13-4</t>
+          <t>Kyle Cochran , (Maryland) DEC John Poznanski , (Rutgers), 7-3</t>
         </is>
       </c>
     </row>
@@ -7722,7 +7722,7 @@
       </c>
       <c r="B615" t="inlineStr">
         <is>
-          <t>Trent Hidlay , (NC State) MD Max Lyon , (Purdue), 12-3</t>
+          <t>Parker Keckeisen , (Northern Iowa) MD Christopher Weiler , (Wisconsin), 13-4</t>
         </is>
       </c>
     </row>
@@ -7734,7 +7734,7 @@
       </c>
       <c r="B616" t="inlineStr">
         <is>
-          <t>Isaiah Salazar , (Minnesota) DEC Gavin Kane , (North Carolina), 7-2</t>
+          <t>Trent Hidlay , (NC State) MD Max Lyon , (Purdue), 12-3</t>
         </is>
       </c>
     </row>
@@ -7746,7 +7746,7 @@
       </c>
       <c r="B617" t="inlineStr">
         <is>
-          <t>Jonathan Loew , (Cornell) DEC Layne Malczewski , (Michigan State), 11-4</t>
+          <t>Isaiah Salazar , (Minnesota) DEC Gavin Kane , (North Carolina), 7-2</t>
         </is>
       </c>
     </row>
@@ -7758,7 +7758,7 @@
       </c>
       <c r="B618" t="inlineStr">
         <is>
-          <t>Trey Munoz , (Oregon State) DEC Keegan Moore , (Oklahoma), 8-3</t>
+          <t>Jonathan Loew , (Cornell) DEC Layne Malczewski , (Michigan State), 11-4</t>
         </is>
       </c>
     </row>
@@ -7770,7 +7770,7 @@
       </c>
       <c r="B619" t="inlineStr">
         <is>
-          <t>Kaleb Romero , (Ohio State) MD Donnell Washington , (Indiana), 13-2</t>
+          <t>Trey Munoz , (Oregon State) DEC Keegan Moore , (Oklahoma), 8-3</t>
         </is>
       </c>
     </row>
@@ -7782,7 +7782,7 @@
       </c>
       <c r="B620" t="inlineStr">
         <is>
-          <t>Taylor Venz , (Nebraska) DEC Travis Stefanik , (Princeton), 9-2</t>
+          <t>Kaleb Romero , (Ohio State) MD Donnell Washington , (Indiana), 13-2</t>
         </is>
       </c>
     </row>
@@ -7794,7 +7794,7 @@
       </c>
       <c r="B621" t="inlineStr">
         <is>
-          <t>Hunter Bolen , (Virginia Tech) DEC Abe Assad , (Iowa), 6-3</t>
+          <t>Taylor Venz , (Nebraska) DEC Travis Stefanik , (Princeton), 9-2</t>
         </is>
       </c>
     </row>
@@ -7806,19 +7806,19 @@
       </c>
       <c r="B622" t="inlineStr">
         <is>
-          <t>Aaron Brooks , (Penn State) MD Aj Burkhart , (Lehigh), 21-7</t>
+          <t>Hunter Bolen , (Virginia Tech) DEC Abe Assad , (Iowa), 6-3</t>
         </is>
       </c>
     </row>
     <row r="623">
       <c r="A623" t="inlineStr">
         <is>
-          <t>197</t>
+          <t>184</t>
         </is>
       </c>
       <c r="B623" t="inlineStr">
         <is>
-          <t>Max Dean , (Penn State) TF William Feldkamp , (Clarion), 17-1</t>
+          <t>Aaron Brooks , (Penn State) MD Aj Burkhart , (Lehigh), 21-7</t>
         </is>
       </c>
     </row>
@@ -7830,7 +7830,7 @@
       </c>
       <c r="B624" t="inlineStr">
         <is>
-          <t>Jay Aiello , (Virginia) DEC Kordell Norfleet , (Arizona State), 5-3 SV</t>
+          <t>Max Dean , (Penn State) TF William Feldkamp , (Clarion), 17-1</t>
         </is>
       </c>
     </row>
@@ -7842,7 +7842,7 @@
       </c>
       <c r="B625" t="inlineStr">
         <is>
-          <t>Cameron Caffey , (Michigan State) DEC Evan Bockman , (Utah Valley), 6-4</t>
+          <t>Jay Aiello , (Virginia) DEC Kordell Norfleet , (Arizona State), 5-3 SV</t>
         </is>
       </c>
     </row>
@@ -7854,7 +7854,7 @@
       </c>
       <c r="B626" t="inlineStr">
         <is>
-          <t>Lou Deprez , (Binghamton) DEC Jaron Smith , (Maryland), 8-2</t>
+          <t>Cameron Caffey , (Michigan State) DEC Evan Bockman , (Utah Valley), 6-4</t>
         </is>
       </c>
     </row>
@@ -7866,7 +7866,7 @@
       </c>
       <c r="B627" t="inlineStr">
         <is>
-          <t>Nino Bonaccorsi , (Pittsburgh) MD Andrew Davison , (Northwestern), 9-0</t>
+          <t>Lou Deprez , (Binghamton) DEC Jaron Smith , (Maryland), 8-2</t>
         </is>
       </c>
     </row>
@@ -7878,7 +7878,7 @@
       </c>
       <c r="B628" t="inlineStr">
         <is>
-          <t>Gavin Hoffman , (Ohio State) DEC Tanner Sloan , (South Dakota State), 6-4 SV</t>
+          <t>Nino Bonaccorsi , (Pittsburgh) MD Andrew Davison , (Northwestern), 9-0</t>
         </is>
       </c>
     </row>
@@ -7890,7 +7890,7 @@
       </c>
       <c r="B629" t="inlineStr">
         <is>
-          <t>Jake Woodley , (Oklahoma) DEC Jacob Koser , (Navy), 5-2</t>
+          <t>Gavin Hoffman , (Ohio State) DEC Tanner Sloan , (South Dakota State), 6-4 SV</t>
         </is>
       </c>
     </row>
@@ -7902,7 +7902,7 @@
       </c>
       <c r="B630" t="inlineStr">
         <is>
-          <t>Patrick Brucki , (Michigan) DEC Benjamin Smith , (Cleveland State), 8-3</t>
+          <t>Jake Woodley , (Oklahoma) DEC Jacob Koser , (Navy), 5-2</t>
         </is>
       </c>
     </row>
@@ -7914,7 +7914,7 @@
       </c>
       <c r="B631" t="inlineStr">
         <is>
-          <t>Eric Schultz , (Nebraska) MD Cole Urbas , (Penn), 15-6</t>
+          <t>Patrick Brucki , (Michigan) DEC Benjamin Smith , (Cleveland State), 8-3</t>
         </is>
       </c>
     </row>
@@ -7926,7 +7926,7 @@
       </c>
       <c r="B632" t="inlineStr">
         <is>
-          <t>Greg Bulsak , (Rutgers) DEC Jacob Cardenas , (Cornell), 7-0</t>
+          <t>Eric Schultz , (Nebraska) MD Cole Urbas , (Penn), 15-6</t>
         </is>
       </c>
     </row>
@@ -7938,7 +7938,7 @@
       </c>
       <c r="B633" t="inlineStr">
         <is>
-          <t>Thomas Penola , (Purdue) DEC Owen Pentz , (North Dakota State), 5-2</t>
+          <t>Greg Bulsak , (Rutgers) DEC Jacob Cardenas , (Cornell), 7-0</t>
         </is>
       </c>
     </row>
@@ -7950,7 +7950,7 @@
       </c>
       <c r="B634" t="inlineStr">
         <is>
-          <t>Jacob Warner , (Iowa) MD Alan Clothier , (Northern Colorado), 8-0</t>
+          <t>Thomas Penola , (Purdue) DEC Owen Pentz , (North Dakota State), 5-2</t>
         </is>
       </c>
     </row>
@@ -7962,7 +7962,7 @@
       </c>
       <c r="B635" t="inlineStr">
         <is>
-          <t>Rocky Elam , (Missouri) DEC Michial Foy , (Minnesota), 5-4</t>
+          <t>Jacob Warner , (Iowa) MD Alan Clothier , (Northern Colorado), 8-0</t>
         </is>
       </c>
     </row>
@@ -7974,7 +7974,7 @@
       </c>
       <c r="B636" t="inlineStr">
         <is>
-          <t>Yonger Bastida , (Iowa State) DEC Braxton Amos , (Wisconsin), 3-2</t>
+          <t>Rocky Elam , (Missouri) DEC Michial Foy , (Minnesota), 5-4</t>
         </is>
       </c>
     </row>
@@ -7986,7 +7986,7 @@
       </c>
       <c r="B637" t="inlineStr">
         <is>
-          <t>Luke Stout , (Princeton) DEC Isaac Trumble , (NC State), 6-4 SV</t>
+          <t>Yonger Bastida , (Iowa State) DEC Braxton Amos , (Wisconsin), 3-2</t>
         </is>
       </c>
     </row>
@@ -7998,19 +7998,19 @@
       </c>
       <c r="B638" t="inlineStr">
         <is>
-          <t>Stephen Buchanan , (Wyoming) DEC J.t. Brown Elyria, OH (Army), 2-0</t>
+          <t>Luke Stout , (Princeton) DEC Isaac Trumble , (NC State), 6-4 SV</t>
         </is>
       </c>
     </row>
     <row r="639">
       <c r="A639" t="inlineStr">
         <is>
-          <t>285</t>
+          <t>197</t>
         </is>
       </c>
       <c r="B639" t="inlineStr">
         <is>
-          <t>Gable Steveson , (Minnesota) TF Tyrell Gordon , (Northern Iowa), 25-10</t>
+          <t>Stephen Buchanan , (Wyoming) DEC J.t. Brown Elyria, OH (Army), 2-0</t>
         </is>
       </c>
     </row>
@@ -8022,7 +8022,7 @@
       </c>
       <c r="B640" t="inlineStr">
         <is>
-          <t>Zach Elam , (Missouri) DEC Trent Hillger , (Wisconsin), 5-4</t>
+          <t>Gable Steveson , (Minnesota) TF Tyrell Gordon , (Northern Iowa), 25-10</t>
         </is>
       </c>
     </row>
@@ -8034,7 +8034,7 @@
       </c>
       <c r="B641" t="inlineStr">
         <is>
-          <t>Lucas Davison , (Northwestern) DEC Sam Schuyler , (Iowa State), 4-0</t>
+          <t>Zach Elam , (Missouri) DEC Trent Hillger , (Wisconsin), 5-4</t>
         </is>
       </c>
     </row>
@@ -8046,7 +8046,7 @@
       </c>
       <c r="B642" t="inlineStr">
         <is>
-          <t>Matt Stencel , (Central Michigan) DEC Isaac Reid , (Lock Haven), 8-2</t>
+          <t>Lucas Davison , (Northwestern) DEC Sam Schuyler , (Iowa State), 4-0</t>
         </is>
       </c>
     </row>
@@ -8058,7 +8058,7 @@
       </c>
       <c r="B643" t="inlineStr">
         <is>
-          <t>Wyatt Hendrickson , (Air Force) F Michael Mcaleavey , (The Citadel), 2:14</t>
+          <t>Matt Stencel , (Central Michigan) DEC Isaac Reid , (Lock Haven), 8-2</t>
         </is>
       </c>
     </row>
@@ -8070,7 +8070,7 @@
       </c>
       <c r="B644" t="inlineStr">
         <is>
-          <t>Christian Lance , (Nebraska) DEC Tyrie Houghton , (NC State), 3-2</t>
+          <t>Wyatt Hendrickson , (Air Force) F Michael Mcaleavey , (The Citadel), 2:14</t>
         </is>
       </c>
     </row>
@@ -8082,7 +8082,7 @@
       </c>
       <c r="B645" t="inlineStr">
         <is>
-          <t>Tate Orndorff , (Ohio State) MD Joe Doyle , (Binghamton), 10-2</t>
+          <t>Christian Lance , (Nebraska) DEC Tyrie Houghton , (NC State), 3-2</t>
         </is>
       </c>
     </row>
@@ -8094,7 +8094,7 @@
       </c>
       <c r="B646" t="inlineStr">
         <is>
-          <t>Greg Kerkvliet , (Penn State) F Brandon Metz , (North Dakota State), 4:17</t>
+          <t>Tate Orndorff , (Ohio State) MD Joe Doyle , (Binghamton), 10-2</t>
         </is>
       </c>
     </row>
@@ -8106,7 +8106,7 @@
       </c>
       <c r="B647" t="inlineStr">
         <is>
-          <t>Tony Cassioppi , (Iowa) DEC Josh Heindselman , (Oklahoma), 4-0</t>
+          <t>Greg Kerkvliet , (Penn State) F Brandon Metz , (North Dakota State), 4:17</t>
         </is>
       </c>
     </row>
@@ -8118,7 +8118,7 @@
       </c>
       <c r="B648" t="inlineStr">
         <is>
-          <t>Luke Luffman , (Illinois) MD Luke Surber , (Oklahoma State), 10-2</t>
+          <t>Tony Cassioppi , (Iowa) DEC Josh Heindselman , (Oklahoma), 4-0</t>
         </is>
       </c>
     </row>
@@ -8130,7 +8130,7 @@
       </c>
       <c r="B649" t="inlineStr">
         <is>
-          <t>Gary Traub , (Oregon State) DEC Aj Nevills , (South Dakota State), 7-4 TB1</t>
+          <t>Luke Luffman , (Illinois) MD Luke Surber , (Oklahoma State), 10-2</t>
         </is>
       </c>
     </row>
@@ -8142,7 +8142,7 @@
       </c>
       <c r="B650" t="inlineStr">
         <is>
-          <t>Jordan Wood , (Lehigh) DEC Michael Wolfgram , (West Virginia), 1-0</t>
+          <t>Gary Traub , (Oregon State) DEC Aj Nevills , (South Dakota State), 7-4 TB1</t>
         </is>
       </c>
     </row>
@@ -8154,7 +8154,7 @@
       </c>
       <c r="B651" t="inlineStr">
         <is>
-          <t>Mason Parris , (Michigan) MD Ben Goldin , (Penn), 17-5</t>
+          <t>Jordan Wood , (Lehigh) DEC Michael Wolfgram , (West Virginia), 1-0</t>
         </is>
       </c>
     </row>
@@ -8166,7 +8166,7 @@
       </c>
       <c r="B652" t="inlineStr">
         <is>
-          <t>Nathan Traxler , (Virginia Tech) DEC Quinn Miller , (Virginia), 6-4 SV</t>
+          <t>Mason Parris , (Michigan) MD Ben Goldin , (Penn), 17-5</t>
         </is>
       </c>
     </row>
@@ -8178,7 +8178,7 @@
       </c>
       <c r="B653" t="inlineStr">
         <is>
-          <t>Lewis Fernandes , (Cornell) DEC Taye Ghadiali , (Campbell), 4-0</t>
+          <t>Nathan Traxler , (Virginia Tech) DEC Quinn Miller , (Virginia), 6-4 SV</t>
         </is>
       </c>
     </row>
@@ -8189,6 +8189,18 @@
         </is>
       </c>
       <c r="B654" t="inlineStr">
+        <is>
+          <t>Lewis Fernandes , (Cornell) DEC Taye Ghadiali , (Campbell), 4-0</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>285</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
         <is>
           <t>Cohlton Schultz , (Arizona State) F Zachary Knighton-ward , (Hofstra), 1:25</t>
         </is>

</xml_diff>